<commit_message>
Added Thermostat Stable version
</commit_message>
<xml_diff>
--- a/unit-sh/shsXl.xlsx
+++ b/unit-sh/shsXl.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="34">
   <si>
     <t>TYPE</t>
   </si>
@@ -45,37 +45,52 @@
     <t>LIGHT</t>
   </si>
   <si>
+    <t>LI001</t>
+  </si>
+  <si>
+    <t>Front Door</t>
+  </si>
+  <si>
+    <t>OFF</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>on, off</t>
+  </si>
+  <si>
+    <t>2025-06-13T11:47:11.159111891+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-06-13T11:48:37.387520220+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
     <t>LI002</t>
   </si>
   <si>
-    <t>BD</t>
-  </si>
-  <si>
-    <t>OFF</t>
-  </si>
-  <si>
-    <t>N/A</t>
-  </si>
-  <si>
-    <t>on, off</t>
-  </si>
-  <si>
-    <t>2025-06-12T19:32:43.290175624+02:00[Europe/Amsterdam]</t>
-  </si>
-  <si>
-    <t>2025-06-12T19:34:53.872474411+02:00[Europe/Amsterdam]</t>
-  </si>
-  <si>
-    <t>LI003</t>
-  </si>
-  <si>
-    <t>FD2</t>
-  </si>
-  <si>
-    <t>2025-06-12T19:32:43.296112133+02:00[Europe/Amsterdam]</t>
-  </si>
-  <si>
-    <t>2025-06-12T19:34:34.013748906+02:00[Europe/Amsterdam]</t>
+    <t>Back Door</t>
+  </si>
+  <si>
+    <t>2025-06-13T11:47:11.164240304+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>THERMOSTAT</t>
+  </si>
+  <si>
+    <t>TH001</t>
+  </si>
+  <si>
+    <t>Basement</t>
+  </si>
+  <si>
+    <t>ON, OFF, TEMP_UP, TEMP_DOWN, STATUS</t>
+  </si>
+  <si>
+    <t>2025-06-13T11:47:27.535414286+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-06-13T11:49:05.957775890+02:00[Europe/Amsterdam]</t>
   </si>
   <si>
     <t>DEVICE ID</t>
@@ -93,19 +108,13 @@
     <t>REPEAT</t>
   </si>
   <si>
-    <t>on</t>
-  </si>
-  <si>
-    <t>2025-06-13 17:00</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>2025-06-13 16:20</t>
-  </si>
-  <si>
-    <t>none</t>
+    <t>TH002</t>
+  </si>
+  <si>
+    <t>Attic</t>
+  </si>
+  <si>
+    <t>2025-06-13T11:52:46.639537196+02:00[Europe/Amsterdam]</t>
   </si>
 </sst>
 </file>
@@ -150,7 +159,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -240,7 +249,65 @@
         <v>19</v>
       </c>
       <c r="I3" t="s" s="0">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="0">
         <v>20</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="C4" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="D4" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="E4" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="F4" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="G4" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="H4" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="I4" t="s" s="0">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>31</v>
+      </c>
+      <c r="C5" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="D5" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="E5" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="F5" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="G5" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="H5" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="I5" t="s" s="0">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -250,7 +317,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -258,52 +325,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="D1" t="s" s="0">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="E1" t="s" s="0">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s" s="0">
-        <v>10</v>
-      </c>
-      <c r="B2" t="s" s="0">
-        <v>11</v>
-      </c>
-      <c r="C2" t="s" s="0">
-        <v>26</v>
-      </c>
-      <c r="D2" t="s" s="0">
-        <v>27</v>
-      </c>
-      <c r="E2" t="s" s="0">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s" s="0">
-        <v>10</v>
-      </c>
-      <c r="B3" t="s" s="0">
-        <v>11</v>
-      </c>
-      <c r="C3" t="s" s="0">
-        <v>26</v>
-      </c>
-      <c r="D3" t="s" s="0">
-        <v>29</v>
-      </c>
-      <c r="E3" t="s" s="0">
         <v>30</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added WASHING_MACHINE, and DRYER device types
</commit_message>
<xml_diff>
--- a/unit-sh/shsXl.xlsx
+++ b/unit-sh/shsXl.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="56">
   <si>
     <t>TYPE</t>
   </si>
@@ -42,6 +42,66 @@
     <t>UPDATED_TS</t>
   </si>
   <si>
+    <t>WASHING_MACHINE</t>
+  </si>
+  <si>
+    <t>WA002</t>
+  </si>
+  <si>
+    <t>FamilyWM</t>
+  </si>
+  <si>
+    <t>OFF</t>
+  </si>
+  <si>
+    <t>UnknownBrand</t>
+  </si>
+  <si>
+    <t>UnknownModel</t>
+  </si>
+  <si>
+    <t>ON, OFF, START, STOP, STATUS</t>
+  </si>
+  <si>
+    <t>2025-06-15T15:51:02.983458937+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>DRYER</t>
+  </si>
+  <si>
+    <t>DR002</t>
+  </si>
+  <si>
+    <t>FamilyDR</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>2025-06-15T15:51:02.988011035+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>WA003</t>
+  </si>
+  <si>
+    <t>BAby</t>
+  </si>
+  <si>
+    <t>2025-06-15T15:51:02.984194029+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>DR003</t>
+  </si>
+  <si>
+    <t>DR3</t>
+  </si>
+  <si>
+    <t>2025-06-15T15:51:02.988358015+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-06-15T15:52:34.391489682+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
     <t>LIGHT</t>
   </si>
   <si>
@@ -51,19 +111,10 @@
     <t>Front Door</t>
   </si>
   <si>
-    <t>OFF</t>
-  </si>
-  <si>
-    <t>N/A</t>
-  </si>
-  <si>
     <t>on, off</t>
   </si>
   <si>
-    <t>2025-06-13T11:47:11.159111891+02:00[Europe/Amsterdam]</t>
-  </si>
-  <si>
-    <t>2025-06-13T11:48:37.387520220+02:00[Europe/Amsterdam]</t>
+    <t>2025-06-15T15:51:02.984976241+02:00[Europe/Amsterdam]</t>
   </si>
   <si>
     <t>LI002</t>
@@ -72,7 +123,16 @@
     <t>Back Door</t>
   </si>
   <si>
-    <t>2025-06-13T11:47:11.164240304+02:00[Europe/Amsterdam]</t>
+    <t>2025-06-15T15:51:02.985384702+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>DR001</t>
+  </si>
+  <si>
+    <t>MyDR</t>
+  </si>
+  <si>
+    <t>2025-06-15T15:51:02.987621897+02:00[Europe/Amsterdam]</t>
   </si>
   <si>
     <t>THERMOSTAT</t>
@@ -87,10 +147,25 @@
     <t>ON, OFF, TEMP_UP, TEMP_DOWN, STATUS</t>
   </si>
   <si>
-    <t>2025-06-13T11:47:27.535414286+02:00[Europe/Amsterdam]</t>
-  </si>
-  <si>
-    <t>2025-06-13T11:49:05.957775890+02:00[Europe/Amsterdam]</t>
+    <t>2025-06-15T15:51:02.985862876+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>TH002</t>
+  </si>
+  <si>
+    <t>Entrence Hall</t>
+  </si>
+  <si>
+    <t>2025-06-15T15:51:02.986656323+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>WA001</t>
+  </si>
+  <si>
+    <t>MyWM</t>
+  </si>
+  <si>
+    <t>2025-06-15T15:51:02.987094155+02:00[Europe/Amsterdam]</t>
   </si>
   <si>
     <t>DEVICE ID</t>
@@ -106,15 +181,6 @@
   </si>
   <si>
     <t>REPEAT</t>
-  </si>
-  <si>
-    <t>TH002</t>
-  </si>
-  <si>
-    <t>Attic</t>
-  </si>
-  <si>
-    <t>2025-06-13T11:52:46.639537196+02:00[Europe/Amsterdam]</t>
   </si>
 </sst>
 </file>
@@ -159,7 +225,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -211,13 +277,13 @@
         <v>13</v>
       </c>
       <c r="F2" t="s" s="0">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G2" t="s" s="0">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H2" t="s" s="0">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I2" t="s" s="0">
         <v>16</v>
@@ -225,42 +291,42 @@
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C3" t="s" s="0">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D3" t="s" s="0">
         <v>12</v>
       </c>
       <c r="E3" t="s" s="0">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="F3" t="s" s="0">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="G3" t="s" s="0">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H3" t="s" s="0">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="I3" t="s" s="0">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C4" t="s" s="0">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D4" t="s" s="0">
         <v>12</v>
@@ -269,45 +335,219 @@
         <v>13</v>
       </c>
       <c r="F4" t="s" s="0">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G4" t="s" s="0">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="H4" t="s" s="0">
         <v>24</v>
       </c>
       <c r="I4" t="s" s="0">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B5" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="C5" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="D5" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="E5" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="F5" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="G5" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="H5" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="I5" t="s" s="0">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="B6" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="C6" t="s" s="0">
         <v>31</v>
       </c>
-      <c r="C5" t="s" s="0">
+      <c r="D6" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="E6" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="F6" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="G6" t="s" s="0">
         <v>32</v>
       </c>
-      <c r="D5" t="s" s="0">
+      <c r="H6" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="I6" t="s" s="0">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="B7" t="s" s="0">
+        <v>34</v>
+      </c>
+      <c r="C7" t="s" s="0">
+        <v>35</v>
+      </c>
+      <c r="D7" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="E7" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="F7" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="G7" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="H7" t="s" s="0">
+        <v>36</v>
+      </c>
+      <c r="I7" t="s" s="0">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="B8" t="s" s="0">
+        <v>37</v>
+      </c>
+      <c r="C8" t="s" s="0">
+        <v>38</v>
+      </c>
+      <c r="D8" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="E8" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="F8" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="G8" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="H8" t="s" s="0">
+        <v>39</v>
+      </c>
+      <c r="I8" t="s" s="0">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s" s="0">
+        <v>40</v>
+      </c>
+      <c r="B9" t="s" s="0">
+        <v>41</v>
+      </c>
+      <c r="C9" t="s" s="0">
+        <v>42</v>
+      </c>
+      <c r="D9" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="E9" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="F9" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="G9" t="s" s="0">
+        <v>43</v>
+      </c>
+      <c r="H9" t="s" s="0">
+        <v>44</v>
+      </c>
+      <c r="I9" t="s" s="0">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s" s="0">
+        <v>40</v>
+      </c>
+      <c r="B10" t="s" s="0">
+        <v>45</v>
+      </c>
+      <c r="C10" t="s" s="0">
+        <v>46</v>
+      </c>
+      <c r="D10" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="E10" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="F10" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="G10" t="s" s="0">
+        <v>43</v>
+      </c>
+      <c r="H10" t="s" s="0">
+        <v>47</v>
+      </c>
+      <c r="I10" t="s" s="0">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s" s="0">
+        <v>48</v>
+      </c>
+      <c r="C11" t="s" s="0">
+        <v>49</v>
+      </c>
+      <c r="D11" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="E11" t="s" s="0">
         <v>13</v>
       </c>
-      <c r="E5" t="s" s="0">
-        <v>13</v>
-      </c>
-      <c r="F5" t="s" s="0">
-        <v>23</v>
-      </c>
-      <c r="G5" t="s" s="0">
-        <v>33</v>
-      </c>
-      <c r="H5" t="s" s="0">
-        <v>33</v>
-      </c>
-      <c r="I5" t="s" s="0">
-        <v>13</v>
+      <c r="F11" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="G11" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="H11" t="s" s="0">
+        <v>50</v>
+      </c>
+      <c r="I11" t="s" s="0">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -325,19 +565,19 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>26</v>
+        <v>51</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>27</v>
+        <v>52</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>28</v>
+        <v>53</v>
       </c>
       <c r="D1" t="s" s="0">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="E1" t="s" s="0">
-        <v>30</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Some tests and gui
</commit_message>
<xml_diff>
--- a/unit-sh/shsXl.xlsx
+++ b/unit-sh/shsXl.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="781" uniqueCount="241">
   <si>
     <t>DEVICE ID</t>
   </si>
@@ -532,6 +532,213 @@
   </si>
   <si>
     <t>2025-07-03T20:54:49.063216528+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-04T09:09:00.968092492+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-04T09:10:26.441276550+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>Philips</t>
+  </si>
+  <si>
+    <t>PLB10025</t>
+  </si>
+  <si>
+    <t>2025-07-04T09:17:14.211367158+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-04T09:19:26.910687484+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-04T09:19:26.921304077+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>Basement</t>
+  </si>
+  <si>
+    <t>2025-07-04T09:42:53.159481430+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-04T09:42:53.432841418+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>Basement_Studio</t>
+  </si>
+  <si>
+    <t>2025-07-04T10:00:52.213043408+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-04T10:00:52.428446455+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>Basement_Studio_Test_Light</t>
+  </si>
+  <si>
+    <t>2025-07-04T10:01:46.358919353+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-04T10:01:46.550883612+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>Basement_Studio_Test</t>
+  </si>
+  <si>
+    <t>2025-07-04T10:04:34.528501542+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-04T10:04:34.736558714+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-04T11:01:46.713762883+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-04T11:01:46.980337075+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-04T11:01:47.114209+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-04T11:06:22.817539566+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-04T11:06:23.046338358+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-04T11:06:23.119768374+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>Bedroom_Thermostat_Test</t>
+  </si>
+  <si>
+    <t>2025-07-04T11:11:42.458125807+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-04T11:11:42.655951460+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-04T11:11:42.745953581+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-04T11:14:03.392428572+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-04T11:14:03.468826138+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-04T11:14:03.559928237+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-04T11:14:03.655777972+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-04T11:14:03.721070146+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-04T11:14:03.794192170+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>BasementDryer_Test</t>
+  </si>
+  <si>
+    <t>2025-07-04T11:14:03.881867482+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-04T11:14:03.956427134+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-04T11:14:04.016417005+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>DEV001</t>
+  </si>
+  <si>
+    <t>TestDevice</t>
+  </si>
+  <si>
+    <t>OFF</t>
+  </si>
+  <si>
+    <t>2025-07-04 12:34</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>ON</t>
+  </si>
+  <si>
+    <t>2025-07-04 12:35</t>
+  </si>
+  <si>
+    <t>2025-07-05 12:35</t>
+  </si>
+  <si>
+    <t>weekly</t>
+  </si>
+  <si>
+    <t>2025-07-04 12:36</t>
+  </si>
+  <si>
+    <t>daily</t>
+  </si>
+  <si>
+    <t>4 errors to this class:LGHT001</t>
+  </si>
+  <si>
+    <t>MyLight</t>
+  </si>
+  <si>
+    <t>2025-07-04T18:42:46.372028042Z</t>
+  </si>
+  <si>
+    <t>2025-07-04T20:54:39.870510489+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-04T20:54:40.237978704+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-05T00:09:32.712396473+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-05T00:09:32.911621010+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-05T00:16:05.738034413+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-05T00:16:05.944801580+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-05T00:22:06.621651760+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-05T00:22:06.822433218+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-05T00:25:28.094793456+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-05T00:25:28.308260173+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-05T00:30:47.288553282+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-05T00:30:47.530912098+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-05T00:31:44.824207681+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-05T00:31:45.009548555+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-05T00:37:46.157958295+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-05T00:37:46.377879102+02:00[Europe/Amsterdam]</t>
   </si>
 </sst>
 </file>
@@ -606,7 +813,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:L37"/>
+  <dimension ref="A1:L38"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -658,22 +865,22 @@
         <v>26</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>27</v>
+        <v>188</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="E2" t="s" s="0">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="F2" t="b" s="0">
         <v>0</v>
       </c>
       <c r="G2" t="n" s="0">
-        <v>1600.0</v>
+        <v>1400.0</v>
       </c>
       <c r="H2" t="n" s="0">
-        <v>1600.0</v>
+        <v>1400.0</v>
       </c>
       <c r="I2" t="s" s="0">
         <v>30</v>
@@ -682,7 +889,7 @@
         <v>31</v>
       </c>
       <c r="K2" t="s" s="0">
-        <v>55</v>
+        <v>203</v>
       </c>
       <c r="L2" t="s" s="0">
         <v>28</v>
@@ -720,7 +927,7 @@
         <v>34</v>
       </c>
       <c r="K3" t="s" s="0">
-        <v>171</v>
+        <v>239</v>
       </c>
       <c r="L3" t="s" s="0">
         <v>28</v>
@@ -1193,19 +1400,19 @@
         <v>96</v>
       </c>
       <c r="D16" t="s" s="0">
-        <v>28</v>
+        <v>174</v>
       </c>
       <c r="E16" t="s" s="0">
-        <v>28</v>
-      </c>
-      <c r="F16" t="s" s="0">
-        <v>29</v>
+        <v>175</v>
+      </c>
+      <c r="F16" t="b" s="0">
+        <v>1</v>
       </c>
       <c r="G16" t="n" s="0">
-        <v>1024.0</v>
+        <v>1400.0</v>
       </c>
       <c r="H16" t="n" s="0">
-        <v>1024.0</v>
+        <v>1400.0</v>
       </c>
       <c r="I16" t="s" s="0">
         <v>30</v>
@@ -1214,7 +1421,7 @@
         <v>97</v>
       </c>
       <c r="K16" t="s" s="0">
-        <v>97</v>
+        <v>240</v>
       </c>
       <c r="L16" t="s" s="0">
         <v>28</v>
@@ -1570,7 +1777,7 @@
         <v>126</v>
       </c>
       <c r="C26" t="s" s="0">
-        <v>127</v>
+        <v>197</v>
       </c>
       <c r="D26" t="s" s="0">
         <v>28</v>
@@ -1578,23 +1785,23 @@
       <c r="E26" t="s" s="0">
         <v>28</v>
       </c>
-      <c r="F26" t="s" s="0">
-        <v>29</v>
+      <c r="F26" t="b" s="0">
+        <v>0</v>
       </c>
       <c r="G26" t="n" s="0">
-        <v>23.0</v>
+        <v>21.0</v>
       </c>
       <c r="H26" t="n" s="0">
-        <v>23.0</v>
+        <v>27.0</v>
       </c>
       <c r="I26" t="s" s="0">
-        <v>128</v>
+        <v>30</v>
       </c>
       <c r="J26" t="s" s="0">
         <v>129</v>
       </c>
       <c r="K26" t="s" s="0">
-        <v>129</v>
+        <v>206</v>
       </c>
       <c r="L26" t="s" s="0">
         <v>28</v>
@@ -1988,7 +2195,7 @@
         <v>165</v>
       </c>
       <c r="C37" t="s" s="0">
-        <v>166</v>
+        <v>207</v>
       </c>
       <c r="D37" t="s" s="0">
         <v>28</v>
@@ -1996,25 +2203,63 @@
       <c r="E37" t="s" s="0">
         <v>28</v>
       </c>
-      <c r="F37" t="s" s="0">
-        <v>29</v>
+      <c r="F37" t="b" s="0">
+        <v>0</v>
       </c>
       <c r="G37" t="n" s="0">
-        <v>0.0</v>
+        <v>1300.0</v>
       </c>
       <c r="H37" t="n" s="0">
-        <v>0.0</v>
+        <v>1300.0</v>
       </c>
       <c r="I37" t="s" s="0">
-        <v>162</v>
+        <v>30</v>
       </c>
       <c r="J37" t="s" s="0">
         <v>167</v>
       </c>
       <c r="K37" t="s" s="0">
-        <v>167</v>
+        <v>210</v>
       </c>
       <c r="L37" t="s" s="0">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="B38" t="s" s="0">
+        <v>222</v>
+      </c>
+      <c r="C38" t="s" s="0">
+        <v>223</v>
+      </c>
+      <c r="D38" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="E38" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="F38" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="G38" t="n" s="0">
+        <v>400.0</v>
+      </c>
+      <c r="H38" t="n" s="0">
+        <v>400.0</v>
+      </c>
+      <c r="I38" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="J38" t="s" s="0">
+        <v>224</v>
+      </c>
+      <c r="K38" t="s" s="0">
+        <v>224</v>
+      </c>
+      <c r="L38" t="s" s="0">
         <v>28</v>
       </c>
     </row>
@@ -2074,7 +2319,7 @@
         <v>37</v>
       </c>
       <c r="E2" t="n" s="0">
-        <v>1399.0</v>
+        <v>1200.0</v>
       </c>
       <c r="F2" t="s" s="0">
         <v>38</v>
@@ -2083,7 +2328,7 @@
         <v>39</v>
       </c>
       <c r="H2" t="s" s="0">
-        <v>169</v>
+        <v>178</v>
       </c>
       <c r="I2" t="s" s="0">
         <v>38</v>
@@ -2096,7 +2341,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2139,6 +2384,26 @@
         <v>1400.0</v>
       </c>
       <c r="F2" t="n" s="0">
+        <v>1400.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>95</v>
+      </c>
+      <c r="C3" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="D3" t="s" s="0">
+        <v>35</v>
+      </c>
+      <c r="E3" t="n" s="0">
+        <v>1400.0</v>
+      </c>
+      <c r="F3" t="n" s="0">
         <v>1400.0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
modular menus, Light redemption, and washer realism
</commit_message>
<xml_diff>
--- a/unit-sh/shsXl.xlsx
+++ b/unit-sh/shsXl.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2219" uniqueCount="547">
   <si>
     <t xml:space="preserve">DEVICE ID</t>
   </si>
@@ -633,6 +633,1038 @@
   </si>
   <si>
     <t>2025-07-05T13:01:53.951884262+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>Basement_Studio_Test</t>
+  </si>
+  <si>
+    <t>2025-07-05T16:35:29.540331931+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-05T16:35:29.795178528+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-05T16:35:29.896007318+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-05T19:21:30.229164235+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-05T19:21:30.375019149+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-05T19:21:30.491856285+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>DEV001</t>
+  </si>
+  <si>
+    <t>TestDevice</t>
+  </si>
+  <si>
+    <t>OFF</t>
+  </si>
+  <si>
+    <t>2025-07-05 19:21</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>ON</t>
+  </si>
+  <si>
+    <t>2025-07-06 19:21</t>
+  </si>
+  <si>
+    <t>weekly</t>
+  </si>
+  <si>
+    <t>2025-07-05 19:22</t>
+  </si>
+  <si>
+    <t>daily</t>
+  </si>
+  <si>
+    <t>2025-07-05T19:23:17.758486759+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-05T19:23:17.877572718+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-05T19:23:17.994240094+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-05 19:23</t>
+  </si>
+  <si>
+    <t>2025-07-06 19:23</t>
+  </si>
+  <si>
+    <t>2025-07-05 19:24</t>
+  </si>
+  <si>
+    <t>2025-07-05T20:25:22.983310286+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-05T20:25:23.124816245+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-05T20:25:23.249536051+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-05 20:25</t>
+  </si>
+  <si>
+    <t>2025-07-06 20:25</t>
+  </si>
+  <si>
+    <t>2025-07-05 20:26</t>
+  </si>
+  <si>
+    <t>2025-07-05T20:38:37.465619932+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-05T20:38:37.616113399+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-05T20:38:37.727582930+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>BasementDryer_Test</t>
+  </si>
+  <si>
+    <t>2025-07-05T20:38:39.075125571+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-05T20:38:39.133532438+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-05T20:38:39.197618228+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-05 20:38</t>
+  </si>
+  <si>
+    <t>2025-07-06 20:38</t>
+  </si>
+  <si>
+    <t>2025-07-05 20:39</t>
+  </si>
+  <si>
+    <t>2025-07-05T20:55:10.861866904+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-05T20:55:10.977186034+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-05T20:55:11.082152221+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-05T20:55:12.227111207+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-05T20:55:12.291169059+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-05T20:55:12.347915766+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-05 20:55</t>
+  </si>
+  <si>
+    <t>2025-07-06 20:55</t>
+  </si>
+  <si>
+    <t>2025-07-05 20:56</t>
+  </si>
+  <si>
+    <t>2025-07-05T21:23:41.977282318+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-05T21:23:42.102315436+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-05T21:23:42.180363528+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-05T21:23:43.306223642+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-05T21:23:43.362824287+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-05T21:23:43.422578233+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-05 21:23</t>
+  </si>
+  <si>
+    <t>2025-07-06 21:23</t>
+  </si>
+  <si>
+    <t>2025-07-05 21:24</t>
+  </si>
+  <si>
+    <t>2025-07-05T21:28:08.391251342+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-05T21:28:08.536956835+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-05T21:28:08.610514567+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-05T21:34:12.024307678+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-05T21:34:12.142101671+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-05T21:34:12.222089243+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-05T21:34:13.386439237+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-05T21:34:13.447005783+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-05T21:34:13.503409722+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-05 21:34</t>
+  </si>
+  <si>
+    <t>2025-07-06 21:34</t>
+  </si>
+  <si>
+    <t>2025-07-05 21:35</t>
+  </si>
+  <si>
+    <t>2025-07-05T21:38:50.735476247+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-05T21:38:50.878651193+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-05T21:38:50.991912421+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-05T21:38:52.217627488+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-05T21:38:52.296094924+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-05T21:38:52.378696701+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-05 21:38</t>
+  </si>
+  <si>
+    <t>2025-07-06 21:38</t>
+  </si>
+  <si>
+    <t>2025-07-05 21:39</t>
+  </si>
+  <si>
+    <t>2025-07-05T21:43:38.609358106+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-05T21:43:38.766639055+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-05T21:43:38.850446233+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-05T21:43:40.042908455+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-05T21:43:40.100584128+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-05T21:43:40.164945587+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-05 21:43</t>
+  </si>
+  <si>
+    <t>2025-07-06 21:43</t>
+  </si>
+  <si>
+    <t>2025-07-05 21:44</t>
+  </si>
+  <si>
+    <t>2025-07-05T21:55:10.995193956+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-05T21:55:11.117869427+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-05T21:55:11.191779142+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-05T22:02:33.637610007+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-05T22:02:33.760866650+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-05T22:02:33.860696353+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-05T22:02:35.036895132+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-05T22:02:35.115127042+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-05T22:02:35.191515145+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-05 22:02</t>
+  </si>
+  <si>
+    <t>2025-07-06 22:02</t>
+  </si>
+  <si>
+    <t>2025-07-05 22:03</t>
+  </si>
+  <si>
+    <t>LIGHT</t>
+  </si>
+  <si>
+    <t>4 errors to this class:LGHT001</t>
+  </si>
+  <si>
+    <t>MyLight</t>
+  </si>
+  <si>
+    <t>2025-07-05T20:16:02.285002954Z</t>
+  </si>
+  <si>
+    <t>2025-07-05T22:16:39.253325291+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-05T22:16:39.493433286+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-05T22:16:39.713602981+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-05T22:19:28.269145359+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-05T22:19:28.492869295+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-05T22:19:28.630857156+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-05T22:19:31.128615077+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-05T22:19:31.307990487+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-05T22:19:31.425653449+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-05 22:19</t>
+  </si>
+  <si>
+    <t>2025-07-06 22:19</t>
+  </si>
+  <si>
+    <t>2025-07-05 22:20</t>
+  </si>
+  <si>
+    <t>2025-07-05T22:21:33.915140095+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-05T22:21:34.147712859+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-05T22:21:34.316732792+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-05T22:21:48.935432986+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-05T22:21:49.040258668+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-05T22:21:49.145885672+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-05 22:21</t>
+  </si>
+  <si>
+    <t>2025-07-06 22:21</t>
+  </si>
+  <si>
+    <t>2025-07-05 22:22</t>
+  </si>
+  <si>
+    <t>2025-07-05T22:53:00.407470426+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-05T22:53:00.625066393+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-05T22:54:17.513710721+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-05T22:54:17.729555107+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-06T08:51:36.107477356+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-06T08:51:36.270839988+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-06T08:51:36.383157959+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-06T08:51:37.813094504+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-06T08:51:37.889736369+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-06T08:51:37.948753558+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-06 08:51</t>
+  </si>
+  <si>
+    <t>2025-07-07 08:51</t>
+  </si>
+  <si>
+    <t>2025-07-06 08:52</t>
+  </si>
+  <si>
+    <t>2025-07-06T09:42:00.242521572+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-06T09:42:00.421724882+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-06T09:42:00.541159355+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-06T09:43:27.030737737+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-06T09:43:27.092482219+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-06T09:43:27.141831479+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-06 09:43</t>
+  </si>
+  <si>
+    <t>2025-07-07 09:43</t>
+  </si>
+  <si>
+    <t>2025-07-06 09:44</t>
+  </si>
+  <si>
+    <t>2025-07-06T09:56:41.946660626+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-06T09:56:42.064689714+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-06T09:56:42.133505564+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-06T09:56:43.333441147+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-06T09:56:43.403183084+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-06T09:56:43.468005838+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-06 09:56</t>
+  </si>
+  <si>
+    <t>2025-07-07 09:56</t>
+  </si>
+  <si>
+    <t>2025-07-06 09:57</t>
+  </si>
+  <si>
+    <t>2025-07-06T09:57:01.854583539+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-06T09:57:01.994982150+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-06T09:57:02.074076863+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-06T09:57:03.394368232+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-06T09:57:03.470167380+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-06T09:57:03.522261170+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-07 09:57</t>
+  </si>
+  <si>
+    <t>2025-07-06 09:58</t>
+  </si>
+  <si>
+    <t>2025-07-06T10:07:38.277945296+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-06T10:07:38.411217621+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-06T10:07:38.533051927+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-06T10:07:39.959288961+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-06T10:07:40.025271553+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-06T10:07:40.076543214+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-06 10:07</t>
+  </si>
+  <si>
+    <t>2025-07-07 10:07</t>
+  </si>
+  <si>
+    <t>2025-07-06 10:08</t>
+  </si>
+  <si>
+    <t>2025-07-06T10:16:36.621564044+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-06T10:16:36.749176063+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-06T10:16:36.823979777+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-06T10:16:38.300884740+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-06T10:16:38.364203768+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-06T10:16:38.424941732+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-06 10:16</t>
+  </si>
+  <si>
+    <t>2025-07-07 10:16</t>
+  </si>
+  <si>
+    <t>2025-07-06 10:17</t>
+  </si>
+  <si>
+    <t>2025-07-06T16:20:38.133547102+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-06T16:20:38.411054681+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-06T16:20:38.597109012+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-06T16:20:41.432810208+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-06T16:20:41.590689098+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-06T16:20:41.746128373+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-06 16:20</t>
+  </si>
+  <si>
+    <t>2025-07-07 16:20</t>
+  </si>
+  <si>
+    <t>2025-07-06 16:21</t>
+  </si>
+  <si>
+    <t>2025-07-06T16:38:10.056197622+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-06T16:38:10.193696619+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-06T16:38:10.296387414+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-06T16:38:11.939479990+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-06T16:38:11.994246525+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-06T16:38:12.061233794+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-06 16:38</t>
+  </si>
+  <si>
+    <t>2025-07-07 16:38</t>
+  </si>
+  <si>
+    <t>2025-07-06 16:39</t>
+  </si>
+  <si>
+    <t>2025-07-06T16:44:21.377552471+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-06T16:44:21.505325915+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-06T16:44:21.607920266+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-06T16:44:22.921781012+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-06T16:44:22.994925265+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-06T16:44:23.050432648+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-06 16:44</t>
+  </si>
+  <si>
+    <t>2025-07-07 16:44</t>
+  </si>
+  <si>
+    <t>2025-07-06 16:45</t>
+  </si>
+  <si>
+    <t>2025-07-06T16:58:25.702019306+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-06T16:58:25.821260277+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-06T16:58:25.939325400+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-06T16:58:27.335358112+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-06T16:58:27.406854467+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-06T16:58:27.472093865+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-06 16:58</t>
+  </si>
+  <si>
+    <t>2025-07-07 16:58</t>
+  </si>
+  <si>
+    <t>2025-07-06 16:59</t>
+  </si>
+  <si>
+    <t>2025-07-06T17:04:29.085262101+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-06T17:04:29.236842231+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-06T17:04:29.345162944+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-06T17:04:30.763574019+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-06T17:04:30.832622199+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-06T17:04:30.891549796+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-06 17:04</t>
+  </si>
+  <si>
+    <t>2025-07-07 17:04</t>
+  </si>
+  <si>
+    <t>2025-07-06 17:05</t>
+  </si>
+  <si>
+    <t>2025-07-06T18:58:32.658958308+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-06T18:58:32.814432921+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-06T18:58:32.894775640+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>Bedroom_Thermostat_Test</t>
+  </si>
+  <si>
+    <t>2025-07-06T18:58:34.469052393+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-06T18:58:34.527870600+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-06T18:58:34.582342523+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-06T18:58:34.783077746+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-06T18:58:34.835884177+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-06T18:58:34.883031747+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-06 18:58</t>
+  </si>
+  <si>
+    <t>2025-07-07 18:58</t>
+  </si>
+  <si>
+    <t>2025-07-06 18:59</t>
+  </si>
+  <si>
+    <t>2025-07-06T18:16:21.699066917Z</t>
+  </si>
+  <si>
+    <t>2025-07-06T20:16:24.543763600+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-06T20:16:24.611718850+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-06T20:16:24.672794369+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-06 20:16</t>
+  </si>
+  <si>
+    <t>2025-07-07 20:16</t>
+  </si>
+  <si>
+    <t>2025-07-06 20:17</t>
+  </si>
+  <si>
+    <t>2025-07-06T20:16:25.291013018+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-06T20:16:25.339899614+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-06T20:16:25.375639072+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-06T20:16:25.758243377+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-06T20:16:25.790975628+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-06T20:16:25.835970284+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-06T18:19:54.602695019Z</t>
+  </si>
+  <si>
+    <t>LGHT001</t>
+  </si>
+  <si>
+    <t>2025-07-06T18:23:28.768898203Z</t>
+  </si>
+  <si>
+    <t>LI001</t>
+  </si>
+  <si>
+    <t>2025-07-06T18:29:10.873677694Z</t>
+  </si>
+  <si>
+    <t>2025-07-06T18:30:15.364387498Z</t>
+  </si>
+  <si>
+    <t>2025-07-06T20:30:18.137061656+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-06T20:30:18.199154179+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-06T20:30:18.248219752+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-06 20:30</t>
+  </si>
+  <si>
+    <t>2025-07-07 20:30</t>
+  </si>
+  <si>
+    <t>2025-07-06 20:31</t>
+  </si>
+  <si>
+    <t>2025-07-06T20:30:18.938259600+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-06T20:30:18.985055881+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-06T20:30:19.026782622+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-06T20:30:19.560653191+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-06T20:30:19.605198639+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-06T20:30:19.649729916+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-06T19:55:39.179382346Z</t>
+  </si>
+  <si>
+    <t>2025-07-06T21:55:41.822874225+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-06T21:55:41.878729053+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-06T21:55:41.937926963+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-06 21:55</t>
+  </si>
+  <si>
+    <t>2025-07-07 21:55</t>
+  </si>
+  <si>
+    <t>2025-07-06 21:56</t>
+  </si>
+  <si>
+    <t>2025-07-06T21:55:42.593628228+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-06T21:55:42.656127941+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-06T21:55:42.713218989+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-06T21:55:43.252628108+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-06T21:55:43.298660151+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-06T21:55:43.353611371+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-06T22:02:28.711063456+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-06T22:02:29.044452805+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-06T23:28:12.365377331+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-06T23:28:12.619487252+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-06T23:36:24.504360312+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-06T23:36:24.699393080+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-06T23:37:27.497383747+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-06T23:37:27.725973842+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-06T23:38:10.540910296+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-06T23:38:10.760716677+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-06T23:42:01.505890479+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-06T23:42:01.710038876+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-06T23:45:37.361389016+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-06T23:45:37.574192671+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-06T23:48:46.862062674+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-06T23:48:47.038371851+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-07T09:36:25.503278768Z</t>
+  </si>
+  <si>
+    <t>2025-07-07T13:06:15.482549833+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-07T13:06:15.799120547+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-07T13:38:19.247734626Z</t>
+  </si>
+  <si>
+    <t>2025-07-07T15:38:25.982930368+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-07T15:38:26.112905144+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-07T15:38:26.286712158+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-07 15:38</t>
+  </si>
+  <si>
+    <t>2025-07-08 15:38</t>
+  </si>
+  <si>
+    <t>2025-07-07 15:39</t>
+  </si>
+  <si>
+    <t>2025-07-07T15:38:28.035589745+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-07T15:38:28.155131102+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-07T15:38:28.273842672+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-07T18:46:57.395224160+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-07T18:46:57.626280603+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-07T19:01:33.491297165+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-07T19:01:33.869998909+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>Staorcase_Main</t>
+  </si>
+  <si>
+    <t>2025-07-07T19:02:11.407752269+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-07T19:02:16.518265777+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-07T19:02:46.867631205+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-07T20:01:52.173027370+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-07T20:01:52.385399396+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-07T20:11:04.817630254+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-07T20:11:05.042119508+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>FamilyWM</t>
+  </si>
+  <si>
+    <t>BWM14025</t>
+  </si>
+  <si>
+    <t>2025-07-07T20:11:29.244571174+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-07T20:11:33.881037163+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-07T20:11:33.926616179+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-07T20:11:48.454200898+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-07T20:21:44.078120244+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-07T20:21:44.288548491+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-07T20:21:51.891093442+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-07T20:21:54.347808412+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-07T20:21:54.401294621+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-07T20:21:54.446412582+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-07T20:22:06.729922880+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-07T20:22:11.735128248+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-07T20:22:11.777090872+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-07T20:22:11.806746141+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-07T20:22:18.355129635+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-07T20:22:27.255069916+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-07T20:22:27.298680926+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-07T20:22:27.336285477+02:00[Europe/Amsterdam]</t>
   </si>
 </sst>
 </file>
@@ -773,7 +1805,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L39"/>
+  <dimension ref="A1:L48"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E37" activeCellId="0" sqref="E37"/>
@@ -827,32 +1859,28 @@
         <v>18</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F2" s="1" t="n">
+        <v>203</v>
+      </c>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="G2" s="1" t="n">
-        <v>1400</v>
+        <v>1400.0</v>
       </c>
       <c r="H2" s="1" t="n">
-        <v>1400</v>
+        <v>1400.0</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>21</v>
+        <v>165</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>22</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>23</v>
+        <v>514</v>
       </c>
       <c r="L2" s="1" t="s">
         <v>20</v>
@@ -891,7 +1919,7 @@
         <v>28</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>201</v>
+        <v>533</v>
       </c>
       <c r="L3" s="1" t="s">
         <v>20</v>
@@ -1323,31 +2351,31 @@
         <v>64</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>65</v>
+        <v>519</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>20</v>
+        <v>179</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>32</v>
+        <v>179</v>
+      </c>
+      <c r="F15" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="G15" s="1" t="n">
-        <v>1024</v>
+        <v>1024.0</v>
       </c>
       <c r="H15" s="1" t="n">
-        <v>1024</v>
+        <v>1024.0</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>21</v>
+        <v>165</v>
       </c>
       <c r="J15" s="1" t="s">
         <v>66</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>66</v>
+        <v>522</v>
       </c>
       <c r="L15" s="1" t="s">
         <v>20</v>
@@ -1386,7 +2414,7 @@
         <v>71</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>202</v>
+        <v>534</v>
       </c>
       <c r="L16" s="1" t="s">
         <v>20</v>
@@ -1742,32 +2770,28 @@
         <v>101</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F26" s="1" t="n">
+        <v>432</v>
+      </c>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="G26" s="1" t="n">
-        <v>21</v>
+        <v>21.0</v>
       </c>
       <c r="H26" s="1" t="n">
-        <v>27</v>
+        <v>27.0</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>21</v>
+        <v>180</v>
       </c>
       <c r="J26" s="1" t="s">
         <v>103</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>104</v>
+        <v>485</v>
       </c>
       <c r="L26" s="1" t="s">
         <v>20</v>
@@ -2123,31 +3147,31 @@
         <v>134</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>135</v>
+        <v>527</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>136</v>
+        <v>172</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="F36" s="1" t="s">
-        <v>32</v>
+        <v>528</v>
+      </c>
+      <c r="F36" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="G36" s="1" t="n">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="H36" s="1" t="n">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>138</v>
+        <v>174</v>
       </c>
       <c r="J36" s="1" t="s">
         <v>139</v>
       </c>
       <c r="K36" s="1" t="s">
-        <v>139</v>
+        <v>546</v>
       </c>
       <c r="L36" s="1" t="s">
         <v>20</v>
@@ -2161,23 +3185,19 @@
         <v>141</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>173</v>
-      </c>
+        <v>235</v>
+      </c>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
       <c r="F37" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="G37" s="1" t="n">
-        <v>0.0</v>
+        <v>1300.0</v>
       </c>
       <c r="H37" s="1" t="n">
-        <v>0.0</v>
+        <v>1300.0</v>
       </c>
       <c r="I37" s="1" t="s">
         <v>174</v>
@@ -2186,7 +3206,7 @@
         <v>144</v>
       </c>
       <c r="K37" s="1" t="s">
-        <v>182</v>
+        <v>508</v>
       </c>
       <c r="L37" s="1" t="s">
         <v>20</v>
@@ -2261,6 +3281,312 @@
         <v>186</v>
       </c>
       <c r="L39" t="s" s="0">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="s" s="0">
+        <v>302</v>
+      </c>
+      <c r="B40" t="s" s="0">
+        <v>303</v>
+      </c>
+      <c r="C40" t="s" s="0">
+        <v>304</v>
+      </c>
+      <c r="D40" s="0"/>
+      <c r="E40" s="0"/>
+      <c r="F40" t="b" s="0">
+        <v>0</v>
+      </c>
+      <c r="G40" t="n" s="0">
+        <v>400.0</v>
+      </c>
+      <c r="H40" t="n" s="0">
+        <v>600.0</v>
+      </c>
+      <c r="I40" t="s" s="0">
+        <v>165</v>
+      </c>
+      <c r="J40" t="s" s="0">
+        <v>305</v>
+      </c>
+      <c r="K40" t="s" s="0">
+        <v>305</v>
+      </c>
+      <c r="L40" t="s" s="0">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="s" s="0">
+        <v>302</v>
+      </c>
+      <c r="B41" t="s" s="0">
+        <v>303</v>
+      </c>
+      <c r="C41" t="s" s="0">
+        <v>304</v>
+      </c>
+      <c r="D41" s="0"/>
+      <c r="E41" s="0"/>
+      <c r="F41" t="b" s="0">
+        <v>0</v>
+      </c>
+      <c r="G41" t="n" s="0">
+        <v>400.0</v>
+      </c>
+      <c r="H41" t="n" s="0">
+        <v>600.0</v>
+      </c>
+      <c r="I41" t="s" s="0">
+        <v>165</v>
+      </c>
+      <c r="J41" t="s" s="0">
+        <v>442</v>
+      </c>
+      <c r="K41" t="s" s="0">
+        <v>442</v>
+      </c>
+      <c r="L41" t="s" s="0">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="s" s="0">
+        <v>302</v>
+      </c>
+      <c r="B42" t="s" s="0">
+        <v>303</v>
+      </c>
+      <c r="C42" t="s" s="0">
+        <v>304</v>
+      </c>
+      <c r="D42" s="0"/>
+      <c r="E42" s="0"/>
+      <c r="F42" t="b" s="0">
+        <v>0</v>
+      </c>
+      <c r="G42" t="n" s="0">
+        <v>400.0</v>
+      </c>
+      <c r="H42" t="n" s="0">
+        <v>600.0</v>
+      </c>
+      <c r="I42" t="s" s="0">
+        <v>165</v>
+      </c>
+      <c r="J42" t="s" s="0">
+        <v>455</v>
+      </c>
+      <c r="K42" t="s" s="0">
+        <v>455</v>
+      </c>
+      <c r="L42" t="s" s="0">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="s" s="0">
+        <v>302</v>
+      </c>
+      <c r="B43" t="s" s="0">
+        <v>456</v>
+      </c>
+      <c r="C43" t="s" s="0">
+        <v>304</v>
+      </c>
+      <c r="D43" s="0"/>
+      <c r="E43" s="0"/>
+      <c r="F43" t="b" s="0">
+        <v>0</v>
+      </c>
+      <c r="G43" t="n" s="0">
+        <v>400.0</v>
+      </c>
+      <c r="H43" t="n" s="0">
+        <v>600.0</v>
+      </c>
+      <c r="I43" t="s" s="0">
+        <v>165</v>
+      </c>
+      <c r="J43" t="s" s="0">
+        <v>457</v>
+      </c>
+      <c r="K43" t="s" s="0">
+        <v>457</v>
+      </c>
+      <c r="L43" t="s" s="0">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="s" s="0">
+        <v>302</v>
+      </c>
+      <c r="B44" t="s" s="0">
+        <v>458</v>
+      </c>
+      <c r="C44" t="s" s="0">
+        <v>304</v>
+      </c>
+      <c r="D44" s="0"/>
+      <c r="E44" s="0"/>
+      <c r="F44" t="b" s="0">
+        <v>0</v>
+      </c>
+      <c r="G44" t="n" s="0">
+        <v>400.0</v>
+      </c>
+      <c r="H44" t="n" s="0">
+        <v>600.0</v>
+      </c>
+      <c r="I44" t="s" s="0">
+        <v>165</v>
+      </c>
+      <c r="J44" t="s" s="0">
+        <v>459</v>
+      </c>
+      <c r="K44" t="s" s="0">
+        <v>459</v>
+      </c>
+      <c r="L44" t="s" s="0">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="s" s="0">
+        <v>302</v>
+      </c>
+      <c r="B45" t="s" s="0">
+        <v>458</v>
+      </c>
+      <c r="C45" t="s" s="0">
+        <v>304</v>
+      </c>
+      <c r="D45" s="0"/>
+      <c r="E45" s="0"/>
+      <c r="F45" t="b" s="0">
+        <v>0</v>
+      </c>
+      <c r="G45" t="n" s="0">
+        <v>400.0</v>
+      </c>
+      <c r="H45" t="n" s="0">
+        <v>600.0</v>
+      </c>
+      <c r="I45" t="s" s="0">
+        <v>165</v>
+      </c>
+      <c r="J45" t="s" s="0">
+        <v>460</v>
+      </c>
+      <c r="K45" t="s" s="0">
+        <v>460</v>
+      </c>
+      <c r="L45" t="s" s="0">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="s" s="0">
+        <v>302</v>
+      </c>
+      <c r="B46" t="s" s="0">
+        <v>458</v>
+      </c>
+      <c r="C46" t="s" s="0">
+        <v>304</v>
+      </c>
+      <c r="D46" s="0"/>
+      <c r="E46" s="0"/>
+      <c r="F46" t="b" s="0">
+        <v>0</v>
+      </c>
+      <c r="G46" t="n" s="0">
+        <v>400.0</v>
+      </c>
+      <c r="H46" t="n" s="0">
+        <v>600.0</v>
+      </c>
+      <c r="I46" t="s" s="0">
+        <v>165</v>
+      </c>
+      <c r="J46" t="s" s="0">
+        <v>473</v>
+      </c>
+      <c r="K46" t="s" s="0">
+        <v>473</v>
+      </c>
+      <c r="L46" t="s" s="0">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="s" s="0">
+        <v>302</v>
+      </c>
+      <c r="B47" t="s" s="0">
+        <v>458</v>
+      </c>
+      <c r="C47" t="s" s="0">
+        <v>304</v>
+      </c>
+      <c r="D47" s="0"/>
+      <c r="E47" s="0"/>
+      <c r="F47" t="b" s="0">
+        <v>0</v>
+      </c>
+      <c r="G47" t="n" s="0">
+        <v>400.0</v>
+      </c>
+      <c r="H47" t="n" s="0">
+        <v>600.0</v>
+      </c>
+      <c r="I47" t="s" s="0">
+        <v>165</v>
+      </c>
+      <c r="J47" t="s" s="0">
+        <v>502</v>
+      </c>
+      <c r="K47" t="s" s="0">
+        <v>502</v>
+      </c>
+      <c r="L47" t="s" s="0">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="s" s="0">
+        <v>302</v>
+      </c>
+      <c r="B48" t="s" s="0">
+        <v>458</v>
+      </c>
+      <c r="C48" t="s" s="0">
+        <v>304</v>
+      </c>
+      <c r="D48" s="0"/>
+      <c r="E48" s="0"/>
+      <c r="F48" t="b" s="0">
+        <v>0</v>
+      </c>
+      <c r="G48" t="n" s="0">
+        <v>400.0</v>
+      </c>
+      <c r="H48" t="n" s="0">
+        <v>600.0</v>
+      </c>
+      <c r="I48" t="s" s="0">
+        <v>165</v>
+      </c>
+      <c r="J48" t="s" s="0">
+        <v>505</v>
+      </c>
+      <c r="K48" t="s" s="0">
+        <v>505</v>
+      </c>
+      <c r="L48" t="s" s="0">
         <v>179</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Some tests, Class-carving and a SmartLight
</commit_message>
<xml_diff>
--- a/unit-sh/shsXl.xlsx
+++ b/unit-sh/shsXl.xlsx
@@ -13,6 +13,7 @@
     <sheet name="Sensors" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="Sense_Control" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="Tasks" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="Smart_Light_Control" r:id="rId8" sheetId="6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2219" uniqueCount="547">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2743" uniqueCount="669">
   <si>
     <t xml:space="preserve">DEVICE ID</t>
   </si>
@@ -1665,6 +1666,372 @@
   </si>
   <si>
     <t>2025-07-07T20:22:27.336285477+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-07T20:42:37.781713638+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-07T20:42:38.149404131+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-07T21:12:00.137627766+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-07T21:12:00.438409688+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-07T21:39:49.575786093+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-07T21:39:49.823439017+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-07T21:43:18.835831368+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-07T21:43:19.066682138+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-07T21:48:27.158540635+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-07T21:48:27.400650315+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>LI015</t>
+  </si>
+  <si>
+    <t>LIs001</t>
+  </si>
+  <si>
+    <t>2025-07-07T21:53:27.503896904+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-07T21:53:27.720225216+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-07T21:54:00.819721851+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-07T22:00:42.337172224+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-07T22:00:42.541892752+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-07T22:01:05.713571728+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-08T08:52:28.905665998+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-08T08:52:29.249308627+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>DR001</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>2025-07-08T08:54:50.954663241+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-08T09:01:46.083173069+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-08T09:01:46.400584663+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-08T09:02:09.468703871+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-08T09:02:18.082211437+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-08T09:02:18.152545327+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-08T09:02:18.204849308+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-08T09:13:48.302071465+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-08T09:13:48.557341523+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-08T09:14:29.255568237+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-08T09:14:33.459323569+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-08T09:14:33.510751395+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-08T09:14:33.547361091+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-08T09:14:46.487711173+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>WA001</t>
+  </si>
+  <si>
+    <t>2025-07-08T09:15:05.953433389+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-08T09:16:25.915740323+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-08T09:16:26.171800912+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>MODE_NAME</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>IS_DEFAULT</t>
+  </si>
+  <si>
+    <t>EFFECT_NAME</t>
+  </si>
+  <si>
+    <t>TYPE</t>
+  </si>
+  <si>
+    <t>PARAMS</t>
+  </si>
+  <si>
+    <t>2025-07-08T11:10:31.775926544+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-08T11:10:32.156011813+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>SMART_LIGHT</t>
+  </si>
+  <si>
+    <t>SM001</t>
+  </si>
+  <si>
+    <t>Audrey's_Smart_Light</t>
+  </si>
+  <si>
+    <t>on, off, status</t>
+  </si>
+  <si>
+    <t>2025-07-08T11:11:44.685319083+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>2025-07-08T11:12:32.907721379+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-08T11:13:00.129635883+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-08T11:13:02.043010059+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-08T12:27:39.514447884+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-08T12:27:39.763304272+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-08T12:32:50.942303319+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-08T12:32:51.161977363+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-08T12:33:18.828911366+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-08T12:35:30.763459736+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-08T12:35:30.958792948+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>SM002</t>
+  </si>
+  <si>
+    <t>BB</t>
+  </si>
+  <si>
+    <t>2025-07-08T12:35:49.501897358+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-08T12:41:47.401527447+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-08T12:41:47.612299529+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-08T12:41:58.834698408+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-08T12:45:29.200631639+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-08T12:45:29.511359757+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>SL001</t>
+  </si>
+  <si>
+    <t>2025-07-08T12:45:47.673197518+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-08T13:11:50.889970164+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-08T13:11:51.110910457+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-08T13:16:30.647035519+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-08T13:16:30.870616686+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-08T13:18:15.804526002+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-08T13:46:47.918983892+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-08T13:46:48.106548144+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-08T13:47:53.244457893+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-08T14:24:58.590642963+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-08T14:24:58.795343985+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-08T14:48:29.428829949+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-08T14:48:29.632662156+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>ASL2</t>
+  </si>
+  <si>
+    <t>2025-07-08T14:48:46.661059400+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-08T14:49:29.179494160+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-08T14:50:04.054435353+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-08T14:54:00.408896637+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-08T14:54:00.945970203+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-08T14:54:17.585034772+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>Calex Light</t>
+  </si>
+  <si>
+    <t>Calex</t>
+  </si>
+  <si>
+    <t>Calex A60E27</t>
+  </si>
+  <si>
+    <t>on, off, setMode, status</t>
+  </si>
+  <si>
+    <t>2025-07-08T15:38:13.263856927+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-08T15:39:29.164258964+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-08T15:47:52.553247500+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-08T15:48:01.119932432+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-08T15:48:23.898712620+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-08T15:48:44.763689004+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-08T15:49:01.415815448+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-08T15:49:11.259986563+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-08T15:58:44.341028968+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-08T16:08:46.842128717+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-08T16:09:46.789028859+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-08T16:13:17.495144517+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-08T21:28:19.600290268+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-08T21:28:19.807904786+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-09T00:00:14.932224266+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-09T00:00:15.013898019+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-09T00:00:15.078798183+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-09 00:00</t>
+  </si>
+  <si>
+    <t>2025-07-10 00:00</t>
+  </si>
+  <si>
+    <t>2025-07-09 00:01</t>
+  </si>
+  <si>
+    <t>2025-07-09T00:00:16.016446291+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-09T00:00:16.065673002+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-09T00:00:16.110652697+02:00[Europe/Amsterdam]</t>
   </si>
 </sst>
 </file>
@@ -1805,7 +2172,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L48"/>
+  <dimension ref="A1:P49"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E37" activeCellId="0" sqref="E37"/>
@@ -1880,7 +2247,7 @@
         <v>22</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>514</v>
+        <v>668</v>
       </c>
       <c r="L2" s="1" t="s">
         <v>20</v>
@@ -1919,7 +2286,7 @@
         <v>28</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>533</v>
+        <v>658</v>
       </c>
       <c r="L3" s="1" t="s">
         <v>20</v>
@@ -2414,7 +2781,7 @@
         <v>71</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>534</v>
+        <v>659</v>
       </c>
       <c r="L16" s="1" t="s">
         <v>20</v>
@@ -3171,7 +3538,7 @@
         <v>139</v>
       </c>
       <c r="K36" s="1" t="s">
-        <v>546</v>
+        <v>584</v>
       </c>
       <c r="L36" s="1" t="s">
         <v>20</v>
@@ -3206,7 +3573,7 @@
         <v>144</v>
       </c>
       <c r="K37" s="1" t="s">
-        <v>508</v>
+        <v>662</v>
       </c>
       <c r="L37" s="1" t="s">
         <v>20</v>
@@ -3588,6 +3955,56 @@
       </c>
       <c r="L48" t="s" s="0">
         <v>179</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="s" s="0">
+        <v>597</v>
+      </c>
+      <c r="B49" t="s" s="0">
+        <v>621</v>
+      </c>
+      <c r="C49" t="s" s="0">
+        <v>642</v>
+      </c>
+      <c r="D49" s="0" t="s">
+        <v>643</v>
+      </c>
+      <c r="E49" s="0" t="s">
+        <v>644</v>
+      </c>
+      <c r="F49" t="b" s="0">
+        <v>0</v>
+      </c>
+      <c r="G49" t="n" s="0">
+        <v>1050.0</v>
+      </c>
+      <c r="H49" t="n" s="0">
+        <v>1050.0</v>
+      </c>
+      <c r="I49" t="s" s="0">
+        <v>645</v>
+      </c>
+      <c r="J49" t="s" s="0">
+        <v>636</v>
+      </c>
+      <c r="K49" t="s" s="0">
+        <v>657</v>
+      </c>
+      <c r="L49" t="s" s="0">
+        <v>179</v>
+      </c>
+      <c r="M49" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="N49" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="O49" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="P49" t="s" s="0">
+        <v>602</v>
       </c>
     </row>
   </sheetData>
@@ -3732,24 +4149,24 @@
         <v>1400</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="E3" s="1" t="n">
-        <v>1400</v>
-      </c>
-      <c r="F3" s="1" t="n">
-        <v>1400</v>
+    <row r="3">
+      <c r="A3" t="s" s="0">
+        <v>302</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>557</v>
+      </c>
+      <c r="C3" t="s" s="0">
+        <v>302</v>
+      </c>
+      <c r="D3" t="s" s="0">
+        <v>558</v>
+      </c>
+      <c r="E3" t="n" s="0">
+        <v>1400.0</v>
+      </c>
+      <c r="F3" t="n" s="0">
+        <v>1400.0</v>
       </c>
     </row>
   </sheetData>
@@ -3802,4 +4219,43 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:H1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s" s="0">
+        <v>587</v>
+      </c>
+      <c r="B1" t="s" s="0">
+        <v>588</v>
+      </c>
+      <c r="C1" t="s" s="0">
+        <v>589</v>
+      </c>
+      <c r="D1" t="s" s="0">
+        <v>590</v>
+      </c>
+      <c r="E1" t="s" s="0">
+        <v>591</v>
+      </c>
+      <c r="F1" t="s" s="0">
+        <v>592</v>
+      </c>
+      <c r="G1" t="s" s="0">
+        <v>593</v>
+      </c>
+      <c r="H1" t="s" s="0">
+        <v>594</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
First full test iteration
</commit_message>
<xml_diff>
--- a/unit-sh/shsXl.xlsx
+++ b/unit-sh/shsXl.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2743" uniqueCount="669">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3054" uniqueCount="728">
   <si>
     <t xml:space="preserve">DEVICE ID</t>
   </si>
@@ -2032,6 +2032,183 @@
   </si>
   <si>
     <t>2025-07-09T00:00:16.110652697+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-09T22:38:52.453496369+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-09T22:38:52.534886287+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-09T22:38:52.598814112+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-09 22:38</t>
+  </si>
+  <si>
+    <t>2025-07-10 22:38</t>
+  </si>
+  <si>
+    <t>2025-07-09 22:39</t>
+  </si>
+  <si>
+    <t>2025-07-09T22:38:53.578276950+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-09T22:38:53.663210513+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-09T22:38:53.745455448+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-09T22:50:21.104708584+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-09T22:50:21.687015474+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>on</t>
+  </si>
+  <si>
+    <t>2025-07-09 22:58</t>
+  </si>
+  <si>
+    <t>2025-07-09T22:58:25.014073243+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-09T22:58:25.093936180+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-10T12:16:59.450154591+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-10T12:16:59.729918525+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-10 17:54</t>
+  </si>
+  <si>
+    <t>2025-07-10 17:55</t>
+  </si>
+  <si>
+    <t>2025-07-11 17:55</t>
+  </si>
+  <si>
+    <t>2025-07-10 17:56</t>
+  </si>
+  <si>
+    <t>2025-07-10T17:55:05.224877647+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-10T17:55:05.303981616+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-10T17:55:05.373487943+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-10 20:04</t>
+  </si>
+  <si>
+    <t>2025-07-11 20:04</t>
+  </si>
+  <si>
+    <t>2025-07-10 20:05</t>
+  </si>
+  <si>
+    <t>2025-07-10T20:04:43.838159103+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-10T20:04:44.098864221+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-10T20:04:44.189782252+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-10T20:04:46.848162463+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-10T20:04:46.919203809+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-10T20:04:46.986054613+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-10T20:04:47.076717358+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-10T20:04:47.156146534+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-10T20:04:47.225441198+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-11 20:05</t>
+  </si>
+  <si>
+    <t>2025-07-10 20:06</t>
+  </si>
+  <si>
+    <t>2025-07-10T20:05:04.473291135+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-10T20:05:04.535654872+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-10T20:05:04.586996441+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-10T20:05:06.028024902+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-10T20:05:06.084820539+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-10T20:05:06.135556280+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-10T20:05:06.408618783+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-10T20:05:06.456805177+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-10T20:05:06.504248965+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-10 20:32</t>
+  </si>
+  <si>
+    <t>2025-07-11 20:32</t>
+  </si>
+  <si>
+    <t>2025-07-10 20:33</t>
+  </si>
+  <si>
+    <t>2025-07-10T20:32:27.819429595+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-10T20:32:27.884149801+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-10T20:32:27.944336134+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-10T20:32:29.763063698+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-10T20:32:29.833152191+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-10T20:32:29.898247690+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-10T20:32:30.250987548+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-10T20:32:30.315811251+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-07-10T20:32:30.372549546+02:00[Europe/Amsterdam]</t>
   </si>
 </sst>
 </file>
@@ -2247,7 +2424,7 @@
         <v>22</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>668</v>
+        <v>727</v>
       </c>
       <c r="L2" s="1" t="s">
         <v>20</v>
@@ -2286,7 +2463,7 @@
         <v>28</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>658</v>
+        <v>684</v>
       </c>
       <c r="L3" s="1" t="s">
         <v>20</v>
@@ -2781,7 +2958,7 @@
         <v>71</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>659</v>
+        <v>685</v>
       </c>
       <c r="L16" s="1" t="s">
         <v>20</v>
@@ -3158,7 +3335,7 @@
         <v>103</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>485</v>
+        <v>721</v>
       </c>
       <c r="L26" s="1" t="s">
         <v>20</v>
@@ -3573,7 +3750,7 @@
         <v>144</v>
       </c>
       <c r="K37" s="1" t="s">
-        <v>662</v>
+        <v>724</v>
       </c>
       <c r="L37" s="1" t="s">
         <v>20</v>
@@ -3967,12 +4144,8 @@
       <c r="C49" t="s" s="0">
         <v>642</v>
       </c>
-      <c r="D49" s="0" t="s">
-        <v>643</v>
-      </c>
-      <c r="E49" s="0" t="s">
-        <v>644</v>
-      </c>
+      <c r="D49" s="0"/>
+      <c r="E49" s="0"/>
       <c r="F49" t="b" s="0">
         <v>0</v>
       </c>
@@ -3983,13 +4156,13 @@
         <v>1050.0</v>
       </c>
       <c r="I49" t="s" s="0">
-        <v>645</v>
+        <v>600</v>
       </c>
       <c r="J49" t="s" s="0">
         <v>636</v>
       </c>
       <c r="K49" t="s" s="0">
-        <v>657</v>
+        <v>683</v>
       </c>
       <c r="L49" t="s" s="0">
         <v>179</v>

</xml_diff>

<commit_message>
Removed stale light state from AutoOp GUI page
</commit_message>
<xml_diff>
--- a/unit-sh/shsXl.xlsx
+++ b/unit-sh/shsXl.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="120">
   <si>
     <t>TASK_ID</t>
   </si>
@@ -145,10 +145,58 @@
     <t>N/A</t>
   </si>
   <si>
-    <t>2025-08-16T11:52:51.305370054+02:00[Europe/Amsterdam]</t>
-  </si>
-  <si>
-    <t>2025-08-16T11:52:51.305432987+02:00[Europe/Amsterdam]</t>
+    <t>2025-08-19T20:52:30.761556212+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-19T20:52:30.761655907+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>LI002</t>
+  </si>
+  <si>
+    <t>Front_Yard</t>
+  </si>
+  <si>
+    <t>2025-08-19T20:52:46.396835172+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-19T20:52:46.396856329+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>LI003</t>
+  </si>
+  <si>
+    <t>Front_Porch</t>
+  </si>
+  <si>
+    <t>2025-08-19T20:53:12.210807087+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-19T20:53:12.210836205+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>LI004</t>
+  </si>
+  <si>
+    <t>Front_Door</t>
+  </si>
+  <si>
+    <t>2025-08-19T20:53:24.819036799+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-19T20:53:24.819082060+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>LITs001</t>
+  </si>
+  <si>
+    <t>FYLS</t>
+  </si>
+  <si>
+    <t>lux</t>
+  </si>
+  <si>
+    <t>2025-08-19T20:53:42.060712863+02:00[Europe/Amsterdam]</t>
   </si>
   <si>
     <t/>
@@ -157,190 +205,178 @@
     <t>ON</t>
   </si>
   <si>
-    <t>2025-08-16T12:58:06.911495724+02:00[Europe/Amsterdam]</t>
-  </si>
-  <si>
-    <t>2025-08-16T12:58:06.911730960+02:00[Europe/Amsterdam]</t>
-  </si>
-  <si>
-    <t>2025-08-16T12:58:06.958674511+02:00[Europe/Amsterdam]</t>
-  </si>
-  <si>
-    <t>2025-08-16T12:58:06.958948788+02:00[Europe/Amsterdam]</t>
-  </si>
-  <si>
-    <t>2025-08-16T13:06:28.684104025+02:00[Europe/Amsterdam]</t>
-  </si>
-  <si>
-    <t>2025-08-16T13:06:28.684367157+02:00[Europe/Amsterdam]</t>
-  </si>
-  <si>
-    <t>2025-08-16T13:06:28.712952443+02:00[Europe/Amsterdam]</t>
-  </si>
-  <si>
-    <t>2025-08-16T13:06:28.713207449+02:00[Europe/Amsterdam]</t>
-  </si>
-  <si>
-    <t>2025-08-16T13:13:53.035167466+02:00[Europe/Amsterdam]</t>
-  </si>
-  <si>
-    <t>2025-08-16T13:13:53.035391157+02:00[Europe/Amsterdam]</t>
-  </si>
-  <si>
-    <t>2025-08-16T13:13:53.088741899+02:00[Europe/Amsterdam]</t>
-  </si>
-  <si>
-    <t>2025-08-16T13:13:53.088953554+02:00[Europe/Amsterdam]</t>
-  </si>
-  <si>
-    <t>2025-08-16T13:20:18.114365252+02:00[Europe/Amsterdam]</t>
-  </si>
-  <si>
-    <t>2025-08-16T13:20:18.114678419+02:00[Europe/Amsterdam]</t>
-  </si>
-  <si>
-    <t>2025-08-16T13:20:18.167845528+02:00[Europe/Amsterdam]</t>
-  </si>
-  <si>
-    <t>2025-08-16T13:20:18.168008351+02:00[Europe/Amsterdam]</t>
-  </si>
-  <si>
-    <t>2025-08-16T13:20:26.735787328+02:00[Europe/Amsterdam]</t>
-  </si>
-  <si>
-    <t>2025-08-16T13:20:26.736094164+02:00[Europe/Amsterdam]</t>
-  </si>
-  <si>
-    <t>2025-08-16T13:20:26.766163646+02:00[Europe/Amsterdam]</t>
-  </si>
-  <si>
-    <t>2025-08-16T13:20:26.766311614+02:00[Europe/Amsterdam]</t>
-  </si>
-  <si>
-    <t>LI002</t>
-  </si>
-  <si>
-    <t>Front_Yard</t>
-  </si>
-  <si>
-    <t>2025-08-16T13:23:54.474865219+02:00[Europe/Amsterdam]</t>
-  </si>
-  <si>
-    <t>2025-08-16T13:23:54.474906915+02:00[Europe/Amsterdam]</t>
-  </si>
-  <si>
-    <t>LI003</t>
-  </si>
-  <si>
-    <t>Front_Path</t>
-  </si>
-  <si>
-    <t>2025-08-16T13:24:40.852565939+02:00[Europe/Amsterdam]</t>
-  </si>
-  <si>
-    <t>2025-08-16T13:24:40.852623783+02:00[Europe/Amsterdam]</t>
-  </si>
-  <si>
-    <t>2025-08-16T13:24:53.753558497+02:00[Europe/Amsterdam]</t>
-  </si>
-  <si>
-    <t>2025-08-16T13:24:53.753671664+02:00[Europe/Amsterdam]</t>
-  </si>
-  <si>
-    <t>2025-08-16T13:25:04.038989104+02:00[Europe/Amsterdam]</t>
-  </si>
-  <si>
-    <t>2025-08-16T13:25:04.039249308+02:00[Europe/Amsterdam]</t>
-  </si>
-  <si>
-    <t>2025-08-16T13:25:04.063114273+02:00[Europe/Amsterdam]</t>
-  </si>
-  <si>
-    <t>2025-08-16T13:25:04.063206715+02:00[Europe/Amsterdam]</t>
-  </si>
-  <si>
-    <t>2025-08-16T13:25:19.817704977+02:00[Europe/Amsterdam]</t>
-  </si>
-  <si>
-    <t>2025-08-16T13:25:19.818064549+02:00[Europe/Amsterdam]</t>
-  </si>
-  <si>
-    <t>2025-08-16T13:25:19.853597026+02:00[Europe/Amsterdam]</t>
-  </si>
-  <si>
-    <t>2025-08-16T13:25:19.853761417+02:00[Europe/Amsterdam]</t>
-  </si>
-  <si>
-    <t>2025-08-16T13:25:23.662965397+02:00[Europe/Amsterdam]</t>
-  </si>
-  <si>
-    <t>2025-08-16T13:25:23.663119979+02:00[Europe/Amsterdam]</t>
-  </si>
-  <si>
-    <t>2025-08-16T13:25:23.696477788+02:00[Europe/Amsterdam]</t>
-  </si>
-  <si>
-    <t>2025-08-16T13:25:23.696674089+02:00[Europe/Amsterdam]</t>
-  </si>
-  <si>
-    <t>2025-08-16T13:25:27.249595218+02:00[Europe/Amsterdam]</t>
-  </si>
-  <si>
-    <t>2025-08-16T13:25:27.249796546+02:00[Europe/Amsterdam]</t>
-  </si>
-  <si>
-    <t>2025-08-16T13:25:27.278639475+02:00[Europe/Amsterdam]</t>
-  </si>
-  <si>
-    <t>2025-08-16T13:25:27.278869366+02:00[Europe/Amsterdam]</t>
-  </si>
-  <si>
-    <t>LI004</t>
-  </si>
-  <si>
-    <t>NOA</t>
-  </si>
-  <si>
-    <t>2025-08-16T13:47:36.861599985+02:00[Europe/Amsterdam]</t>
-  </si>
-  <si>
-    <t>2025-08-16T13:47:36.861633405+02:00[Europe/Amsterdam]</t>
-  </si>
-  <si>
-    <t>2025-08-16T13:47:59.039337179+02:00[Europe/Amsterdam]</t>
-  </si>
-  <si>
-    <t>2025-08-16T13:47:59.039632115+02:00[Europe/Amsterdam]</t>
-  </si>
-  <si>
-    <t>2025-08-16T13:47:59.063556226+02:00[Europe/Amsterdam]</t>
-  </si>
-  <si>
-    <t>2025-08-16T13:47:59.063684009+02:00[Europe/Amsterdam]</t>
-  </si>
-  <si>
-    <t>2025-08-16T13:48:02.733827731+02:00[Europe/Amsterdam]</t>
-  </si>
-  <si>
-    <t>2025-08-16T13:48:02.733976924+02:00[Europe/Amsterdam]</t>
-  </si>
-  <si>
-    <t>2025-08-16T13:48:02.747194561+02:00[Europe/Amsterdam]</t>
-  </si>
-  <si>
-    <t>2025-08-16T13:48:02.747313249+02:00[Europe/Amsterdam]</t>
-  </si>
-  <si>
-    <t>2025-08-16T13:48:10.351218572+02:00[Europe/Amsterdam]</t>
-  </si>
-  <si>
-    <t>2025-08-16T13:48:10.351438919+02:00[Europe/Amsterdam]</t>
-  </si>
-  <si>
-    <t>2025-08-16T13:48:10.372871590+02:00[Europe/Amsterdam]</t>
-  </si>
-  <si>
-    <t>2025-08-16T13:48:10.372961985+02:00[Europe/Amsterdam]</t>
+    <t>2025-08-19T20:54:07.895082251+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-19T20:54:07.895372843+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-19T20:54:07.944157874+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-19T20:54:07.944396545+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-19T20:54:09.614958808+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-19T20:54:09.615189929+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-19T20:54:09.647790312+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-19T20:54:09.648002138+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-19T20:54:27.364423155+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-19T20:54:27.364594123+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-19T20:54:27.398235838+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-19T20:54:27.398493908+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-19T21:27:59.331676556+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-19T21:27:59.331931583+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-19T21:28:06.655950652+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-19T21:28:06.656094979+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-19T21:28:06.706966146+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-19T21:28:06.707218980+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-19T21:28:09.869257615+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-19T21:28:09.869588892+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>OFF, ON, STATUS</t>
+  </si>
+  <si>
+    <t>2025-08-19T21:44:00.702800706+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-19T21:44:00.703082100+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-19T21:43:46.106431803+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-19T21:44:00.826239630+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-19T21:44:00.826434285+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-19T22:45:11.999084734+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-19T22:45:11.999236770+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-19T22:45:28.478945514+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-19T22:45:28.479008685+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-19T22:45:28.489471836+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-19T22:45:28.489555866+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-19T22:49:28.943378135+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-19T22:49:28.943571562+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-19T22:45:38.161596976+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-19T22:49:29.028390515+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-19T22:49:29.028544289+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-19T22:59:15.712793913+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-19T22:59:15.713068576+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-19T22:59:15.747686988+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-19T22:59:15.747844998+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-19T22:59:17.112658374+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-19T22:59:17.112785344+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-19T22:59:17.150064491+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-19T22:59:17.150299325+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-19T22:59:21.139694039+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-19T22:59:21.139847142+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-19T22:59:02.678742134+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-19T22:59:21.216871629+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-19T22:59:21.216981163+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-19T23:12:50.826670234+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-19T23:12:50.826953379+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-19T23:02:07.601421223+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-19T23:13:57.443977057+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-19T23:13:57.444212049+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-19T23:12:58.458594362+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-19T23:13:57.555784846+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-19T23:13:57.555975735+02:00[Europe/Amsterdam]</t>
   </si>
 </sst>
 </file>
@@ -485,7 +521,7 @@
         <v>38</v>
       </c>
       <c r="F2" t="b" s="0">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G2" t="n" s="0">
         <v>1024.0</v>
@@ -494,19 +530,19 @@
         <v>1024.0</v>
       </c>
       <c r="I2" t="s" s="0">
-        <v>44</v>
+        <v>82</v>
       </c>
       <c r="J2" t="s" s="0">
-        <v>40</v>
+        <v>61</v>
       </c>
       <c r="K2" t="s" s="0">
-        <v>82</v>
+        <v>97</v>
       </c>
       <c r="L2" t="s" s="0">
-        <v>83</v>
+        <v>98</v>
       </c>
       <c r="M2" t="s" s="0">
-        <v>44</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3">
@@ -514,10 +550,10 @@
         <v>34</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>66</v>
+        <v>44</v>
       </c>
       <c r="C3" t="s" s="0">
-        <v>67</v>
+        <v>45</v>
       </c>
       <c r="D3" t="s" s="0">
         <v>37</v>
@@ -526,7 +562,7 @@
         <v>38</v>
       </c>
       <c r="F3" t="b" s="0">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G3" t="n" s="0">
         <v>1024.0</v>
@@ -535,19 +571,19 @@
         <v>1024.0</v>
       </c>
       <c r="I3" t="s" s="0">
-        <v>44</v>
+        <v>82</v>
       </c>
       <c r="J3" t="s" s="0">
-        <v>45</v>
+        <v>61</v>
       </c>
       <c r="K3" t="s" s="0">
-        <v>86</v>
+        <v>118</v>
       </c>
       <c r="L3" t="s" s="0">
-        <v>87</v>
+        <v>119</v>
       </c>
       <c r="M3" t="s" s="0">
-        <v>44</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4">
@@ -555,10 +591,10 @@
         <v>34</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>70</v>
+        <v>48</v>
       </c>
       <c r="C4" t="s" s="0">
-        <v>71</v>
+        <v>49</v>
       </c>
       <c r="D4" t="s" s="0">
         <v>37</v>
@@ -567,7 +603,7 @@
         <v>38</v>
       </c>
       <c r="F4" t="b" s="0">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G4" t="n" s="0">
         <v>1024.0</v>
@@ -576,19 +612,19 @@
         <v>1024.0</v>
       </c>
       <c r="I4" t="s" s="0">
-        <v>44</v>
+        <v>82</v>
       </c>
       <c r="J4" t="s" s="0">
-        <v>40</v>
+        <v>61</v>
       </c>
       <c r="K4" t="s" s="0">
-        <v>90</v>
+        <v>112</v>
       </c>
       <c r="L4" t="s" s="0">
-        <v>91</v>
+        <v>113</v>
       </c>
       <c r="M4" t="s" s="0">
-        <v>44</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5">
@@ -596,10 +632,10 @@
         <v>34</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>92</v>
+        <v>52</v>
       </c>
       <c r="C5" t="s" s="0">
-        <v>93</v>
+        <v>53</v>
       </c>
       <c r="D5" t="s" s="0">
         <v>37</v>
@@ -617,19 +653,19 @@
         <v>1024.0</v>
       </c>
       <c r="I5" t="s" s="0">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="J5" t="s" s="0">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="K5" t="s" s="0">
-        <v>106</v>
+        <v>54</v>
       </c>
       <c r="L5" t="s" s="0">
-        <v>107</v>
+        <v>55</v>
       </c>
       <c r="M5" t="s" s="0">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -693,7 +729,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -725,6 +761,32 @@
         <v>18</v>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="s" s="0">
+        <v>34</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>56</v>
+      </c>
+      <c r="C2" t="s" s="0">
+        <v>57</v>
+      </c>
+      <c r="D2" t="s" s="0">
+        <v>58</v>
+      </c>
+      <c r="E2" t="n" s="0">
+        <v>569.0</v>
+      </c>
+      <c r="F2" t="s" s="0">
+        <v>59</v>
+      </c>
+      <c r="G2" t="s" s="0">
+        <v>59</v>
+      </c>
+      <c r="H2" t="s" s="0">
+        <v>41</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -732,7 +794,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -762,6 +824,75 @@
       </c>
       <c r="H1" t="s" s="0">
         <v>17</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s" s="0">
+        <v>35</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>36</v>
+      </c>
+      <c r="C2" t="n" s="0">
+        <v>1024.0</v>
+      </c>
+      <c r="D2" t="n" s="0">
+        <v>569.0</v>
+      </c>
+      <c r="E2" t="s" s="0">
+        <v>57</v>
+      </c>
+      <c r="F2" t="s" s="0">
+        <v>56</v>
+      </c>
+      <c r="G2" t="s" s="0">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="0">
+        <v>48</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>49</v>
+      </c>
+      <c r="C3" t="n" s="0">
+        <v>1024.0</v>
+      </c>
+      <c r="D3" t="n" s="0">
+        <v>569.0</v>
+      </c>
+      <c r="E3" t="s" s="0">
+        <v>57</v>
+      </c>
+      <c r="F3" t="s" s="0">
+        <v>56</v>
+      </c>
+      <c r="G3" t="s" s="0">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="0">
+        <v>44</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>45</v>
+      </c>
+      <c r="C4" t="n" s="0">
+        <v>1024.0</v>
+      </c>
+      <c r="D4" t="n" s="0">
+        <v>569.0</v>
+      </c>
+      <c r="E4" t="s" s="0">
+        <v>57</v>
+      </c>
+      <c r="F4" t="s" s="0">
+        <v>56</v>
+      </c>
+      <c r="G4" t="s" s="0">
+        <v>117</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Improved GUI AutoOp and device test performence
</commit_message>
<xml_diff>
--- a/unit-sh/shsXl.xlsx
+++ b/unit-sh/shsXl.xlsx
@@ -11,13 +11,12 @@
     <sheet name="Smart_Light_Control" r:id="rId5" sheetId="3"/>
     <sheet name="Sensors" r:id="rId6" sheetId="4"/>
     <sheet name="Sens_Ctrl" r:id="rId7" sheetId="5"/>
-    <sheet name="AutoOp_Ctrl" r:id="rId8" sheetId="6"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="761" uniqueCount="201">
   <si>
     <t>TASK_ID</t>
   </si>
@@ -127,7 +126,7 @@
     <t>LI001</t>
   </si>
   <si>
-    <t>Front_Gate</t>
+    <t>Fornt_Gate</t>
   </si>
   <si>
     <t>Osram</t>
@@ -145,46 +144,58 @@
     <t>N/A</t>
   </si>
   <si>
-    <t>2025-08-19T20:52:30.761556212+02:00[Europe/Amsterdam]</t>
-  </si>
-  <si>
-    <t>2025-08-19T20:52:30.761655907+02:00[Europe/Amsterdam]</t>
+    <t>2025-08-21T13:35:29.112645291+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-21T13:35:29.112943373+02:00[Europe/Amsterdam]</t>
   </si>
   <si>
     <t>LI002</t>
   </si>
   <si>
-    <t>Front_Yard</t>
-  </si>
-  <si>
-    <t>2025-08-19T20:52:46.396835172+02:00[Europe/Amsterdam]</t>
-  </si>
-  <si>
-    <t>2025-08-19T20:52:46.396856329+02:00[Europe/Amsterdam]</t>
+    <t>Fornt_Yard</t>
+  </si>
+  <si>
+    <t>2025-08-21T13:36:47.656195594+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-21T13:36:47.656271173+02:00[Europe/Amsterdam]</t>
   </si>
   <si>
     <t>LI003</t>
   </si>
   <si>
-    <t>Front_Porch</t>
-  </si>
-  <si>
-    <t>2025-08-19T20:53:12.210807087+02:00[Europe/Amsterdam]</t>
-  </si>
-  <si>
-    <t>2025-08-19T20:53:12.210836205+02:00[Europe/Amsterdam]</t>
+    <t>Fornt_</t>
+  </si>
+  <si>
+    <t>2025-08-21T13:37:06.998679477+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-21T13:37:06.998730112+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>Fornt_Porch</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>2025-08-21T13:37:29.775551941+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-21T13:37:29.775896284+02:00[Europe/Amsterdam]</t>
   </si>
   <si>
     <t>LI004</t>
   </si>
   <si>
-    <t>Front_Door</t>
-  </si>
-  <si>
-    <t>2025-08-19T20:53:24.819036799+02:00[Europe/Amsterdam]</t>
-  </si>
-  <si>
-    <t>2025-08-19T20:53:24.819082060+02:00[Europe/Amsterdam]</t>
+    <t>Fornt_Door</t>
+  </si>
+  <si>
+    <t>2025-08-21T13:39:00.263070553+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-21T13:39:00.263165990+02:00[Europe/Amsterdam]</t>
   </si>
   <si>
     <t>LITs001</t>
@@ -196,187 +207,418 @@
     <t>lux</t>
   </si>
   <si>
-    <t>2025-08-19T20:53:42.060712863+02:00[Europe/Amsterdam]</t>
-  </si>
-  <si>
-    <t/>
+    <t>2025-08-21T13:39:24.122768466+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>LITs002</t>
+  </si>
+  <si>
+    <t>BYLS</t>
+  </si>
+  <si>
+    <t>2025-08-21T13:39:38.272216840+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>OFF, ON, STATUS</t>
+  </si>
+  <si>
+    <t>2025-08-21T13:41:48.005708790+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-21T13:41:48.007114566+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-21T13:39:58.577659209+02:00[Europe/Amsterdam]</t>
   </si>
   <si>
     <t>ON</t>
   </si>
   <si>
-    <t>2025-08-19T20:54:07.895082251+02:00[Europe/Amsterdam]</t>
-  </si>
-  <si>
-    <t>2025-08-19T20:54:07.895372843+02:00[Europe/Amsterdam]</t>
-  </si>
-  <si>
-    <t>2025-08-19T20:54:07.944157874+02:00[Europe/Amsterdam]</t>
-  </si>
-  <si>
-    <t>2025-08-19T20:54:07.944396545+02:00[Europe/Amsterdam]</t>
-  </si>
-  <si>
-    <t>2025-08-19T20:54:09.614958808+02:00[Europe/Amsterdam]</t>
-  </si>
-  <si>
-    <t>2025-08-19T20:54:09.615189929+02:00[Europe/Amsterdam]</t>
-  </si>
-  <si>
-    <t>2025-08-19T20:54:09.647790312+02:00[Europe/Amsterdam]</t>
-  </si>
-  <si>
-    <t>2025-08-19T20:54:09.648002138+02:00[Europe/Amsterdam]</t>
-  </si>
-  <si>
-    <t>2025-08-19T20:54:27.364423155+02:00[Europe/Amsterdam]</t>
-  </si>
-  <si>
-    <t>2025-08-19T20:54:27.364594123+02:00[Europe/Amsterdam]</t>
-  </si>
-  <si>
-    <t>2025-08-19T20:54:27.398235838+02:00[Europe/Amsterdam]</t>
-  </si>
-  <si>
-    <t>2025-08-19T20:54:27.398493908+02:00[Europe/Amsterdam]</t>
-  </si>
-  <si>
-    <t>2025-08-19T21:27:59.331676556+02:00[Europe/Amsterdam]</t>
-  </si>
-  <si>
-    <t>2025-08-19T21:27:59.331931583+02:00[Europe/Amsterdam]</t>
-  </si>
-  <si>
-    <t>2025-08-19T21:28:06.655950652+02:00[Europe/Amsterdam]</t>
-  </si>
-  <si>
-    <t>2025-08-19T21:28:06.656094979+02:00[Europe/Amsterdam]</t>
-  </si>
-  <si>
-    <t>2025-08-19T21:28:06.706966146+02:00[Europe/Amsterdam]</t>
-  </si>
-  <si>
-    <t>2025-08-19T21:28:06.707218980+02:00[Europe/Amsterdam]</t>
-  </si>
-  <si>
-    <t>2025-08-19T21:28:09.869257615+02:00[Europe/Amsterdam]</t>
-  </si>
-  <si>
-    <t>2025-08-19T21:28:09.869588892+02:00[Europe/Amsterdam]</t>
-  </si>
-  <si>
-    <t>OFF, ON, STATUS</t>
-  </si>
-  <si>
-    <t>2025-08-19T21:44:00.702800706+02:00[Europe/Amsterdam]</t>
-  </si>
-  <si>
-    <t>2025-08-19T21:44:00.703082100+02:00[Europe/Amsterdam]</t>
-  </si>
-  <si>
-    <t>2025-08-19T21:43:46.106431803+02:00[Europe/Amsterdam]</t>
-  </si>
-  <si>
-    <t>2025-08-19T21:44:00.826239630+02:00[Europe/Amsterdam]</t>
-  </si>
-  <si>
-    <t>2025-08-19T21:44:00.826434285+02:00[Europe/Amsterdam]</t>
-  </si>
-  <si>
-    <t>2025-08-19T22:45:11.999084734+02:00[Europe/Amsterdam]</t>
-  </si>
-  <si>
-    <t>2025-08-19T22:45:11.999236770+02:00[Europe/Amsterdam]</t>
-  </si>
-  <si>
-    <t>2025-08-19T22:45:28.478945514+02:00[Europe/Amsterdam]</t>
-  </si>
-  <si>
-    <t>2025-08-19T22:45:28.479008685+02:00[Europe/Amsterdam]</t>
-  </si>
-  <si>
-    <t>2025-08-19T22:45:28.489471836+02:00[Europe/Amsterdam]</t>
-  </si>
-  <si>
-    <t>2025-08-19T22:45:28.489555866+02:00[Europe/Amsterdam]</t>
-  </si>
-  <si>
-    <t>2025-08-19T22:49:28.943378135+02:00[Europe/Amsterdam]</t>
-  </si>
-  <si>
-    <t>2025-08-19T22:49:28.943571562+02:00[Europe/Amsterdam]</t>
-  </si>
-  <si>
-    <t>2025-08-19T22:45:38.161596976+02:00[Europe/Amsterdam]</t>
-  </si>
-  <si>
-    <t>2025-08-19T22:49:29.028390515+02:00[Europe/Amsterdam]</t>
-  </si>
-  <si>
-    <t>2025-08-19T22:49:29.028544289+02:00[Europe/Amsterdam]</t>
-  </si>
-  <si>
-    <t>2025-08-19T22:59:15.712793913+02:00[Europe/Amsterdam]</t>
-  </si>
-  <si>
-    <t>2025-08-19T22:59:15.713068576+02:00[Europe/Amsterdam]</t>
-  </si>
-  <si>
-    <t>2025-08-19T22:59:15.747686988+02:00[Europe/Amsterdam]</t>
-  </si>
-  <si>
-    <t>2025-08-19T22:59:15.747844998+02:00[Europe/Amsterdam]</t>
-  </si>
-  <si>
-    <t>2025-08-19T22:59:17.112658374+02:00[Europe/Amsterdam]</t>
-  </si>
-  <si>
-    <t>2025-08-19T22:59:17.112785344+02:00[Europe/Amsterdam]</t>
-  </si>
-  <si>
-    <t>2025-08-19T22:59:17.150064491+02:00[Europe/Amsterdam]</t>
-  </si>
-  <si>
-    <t>2025-08-19T22:59:17.150299325+02:00[Europe/Amsterdam]</t>
-  </si>
-  <si>
-    <t>2025-08-19T22:59:21.139694039+02:00[Europe/Amsterdam]</t>
-  </si>
-  <si>
-    <t>2025-08-19T22:59:21.139847142+02:00[Europe/Amsterdam]</t>
-  </si>
-  <si>
-    <t>2025-08-19T22:59:02.678742134+02:00[Europe/Amsterdam]</t>
-  </si>
-  <si>
-    <t>2025-08-19T22:59:21.216871629+02:00[Europe/Amsterdam]</t>
-  </si>
-  <si>
-    <t>2025-08-19T22:59:21.216981163+02:00[Europe/Amsterdam]</t>
-  </si>
-  <si>
-    <t>2025-08-19T23:12:50.826670234+02:00[Europe/Amsterdam]</t>
-  </si>
-  <si>
-    <t>2025-08-19T23:12:50.826953379+02:00[Europe/Amsterdam]</t>
-  </si>
-  <si>
-    <t>2025-08-19T23:02:07.601421223+02:00[Europe/Amsterdam]</t>
-  </si>
-  <si>
-    <t>2025-08-19T23:13:57.443977057+02:00[Europe/Amsterdam]</t>
-  </si>
-  <si>
-    <t>2025-08-19T23:13:57.444212049+02:00[Europe/Amsterdam]</t>
-  </si>
-  <si>
-    <t>2025-08-19T23:12:58.458594362+02:00[Europe/Amsterdam]</t>
-  </si>
-  <si>
-    <t>2025-08-19T23:13:57.555784846+02:00[Europe/Amsterdam]</t>
-  </si>
-  <si>
-    <t>2025-08-19T23:13:57.555975735+02:00[Europe/Amsterdam]</t>
+    <t>2025-08-21T13:41:48.442309241+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-21T13:41:48.442776800+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-21T13:43:10.372852011+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-21T13:43:10.373198487+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-21T13:43:13.516839630+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-21T13:43:13.517088168+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-21T13:44:14.149141553+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-21T13:44:14.149425940+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-21T13:44:14.181024282+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-21T13:44:14.181215866+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-21T13:44:15.415665017+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-21T13:44:15.415904288+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-21T13:44:15.445717818+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-21T13:44:15.445874956+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-21T13:44:20.230715760+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-21T13:44:20.230847103+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-21T13:43:37.933431530+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-21T13:44:20.311768911+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-21T13:44:20.311890113+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-21T13:44:46.273449062+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-21T13:44:46.273665375+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-21T13:45:15.836464039+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-21T13:45:15.836786407+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-21T13:45:15.885776258+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-21T13:45:15.886052147+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-21T13:45:36.264946413+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-21T13:45:36.265170540+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-21T13:44:56.493146140+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-21T13:45:36.362234153+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-21T13:45:36.362362834+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-21T13:46:00.994696346+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-21T13:46:00.994894280+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-21T13:46:21.437070570+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-21T13:46:21.437323903+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-21T13:46:21.468127750+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-21T13:46:21.468289070+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-21T13:46:23.747902664+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-21T13:46:23.748105756+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-21T13:46:13.444927801+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-21T13:46:23.855783028+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-21T13:46:23.855951191+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-21T13:46:43.560762616+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-21T13:46:43.560983632+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-21T13:46:48.553103714+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-21T13:46:48.553428489+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-21T13:46:48.585086185+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-21T13:46:48.585237813+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-21T13:47:18.335162705+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-21T13:47:18.335406040+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-21T13:46:55.958802427+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-21T13:47:18.454380274+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-21T13:47:18.454567184+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-21T13:47:27.766356604+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-21T13:47:27.766508270+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-21T13:46:55.959796108+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-21T14:23:03.709333483+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-21T14:23:03.709499570+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-21T14:23:03.728913062+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-21T14:23:03.729018457+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-21T14:23:07.300967132+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-21T14:23:07.301049512+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-21T14:23:07.317352843+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-21T14:23:07.317429069+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-21T16:18:05.300867233+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-21T16:18:05.301147165+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-21T16:18:10.343623045+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-21T16:18:10.343826061+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-21T16:18:25.671646762+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-21T16:18:25.671821653+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-21T16:18:25.707945922+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-21T16:18:25.708098254+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-21T16:19:03.211853506+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-21T16:19:03.211947546+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-21T16:19:03.236342+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-21T16:19:03.236490244+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-21T16:19:21.995442604+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-21T16:19:21.995573195+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-21T16:17:24.123029947+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-21T16:19:22.061889916+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-21T16:19:22.062013490+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-21T16:47:55.767878031+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-21T16:47:55.768206342+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-21T16:48:29.458566607+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-21T16:48:29.458769575+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-21T16:48:29.498127330+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-21T16:48:29.498306991+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-21T16:48:35.205141835+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-21T16:48:35.205381496+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-21T16:48:17.622089981+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-21T16:48:35.324431826+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-21T16:48:35.324561791+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-21T16:48:57.344764872+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-21T16:48:57.344927886+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-21T16:49:29.684081001+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-21T16:49:29.684352186+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-21T16:49:29.719941531+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-21T16:49:29.720152736+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-21T16:50:08.779324680+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-21T16:50:08.779637338+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-21T16:49:52.882051936+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-21T16:50:08.955119422+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-21T16:50:08.955364865+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-21T18:22:19.258591746+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-21T18:22:19.258965246+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-21T18:22:19.298826605+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-21T18:22:19.298981209+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-21T18:22:20.628012410+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-21T18:22:20.628200271+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-21T18:22:20.662280018+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-21T18:22:20.662479657+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-21T18:22:34.409413481+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-21T18:22:34.409501118+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-21T18:24:01.885339216+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-21T18:24:01.885565083+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-21T18:24:01.926032840+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-21T18:24:01.926213085+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-21T18:24:12.668052554+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-21T18:24:12.668255771+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-21T18:23:34.475403519+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-21T18:24:12.779020201+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-21T18:24:12.779155009+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-21T18:30:12.920613725+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-21T18:30:12.920775953+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-21T18:30:12.947449858+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-21T18:30:12.947633808+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-21T18:30:14.121672343+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-21T18:30:14.121816184+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-21T18:30:14.140905719+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-21T18:30:14.141057925+02:00[Europe/Amsterdam]</t>
   </si>
 </sst>
 </file>
@@ -530,19 +772,19 @@
         <v>1024.0</v>
       </c>
       <c r="I2" t="s" s="0">
-        <v>82</v>
+        <v>67</v>
       </c>
       <c r="J2" t="s" s="0">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="K2" t="s" s="0">
-        <v>97</v>
+        <v>122</v>
       </c>
       <c r="L2" t="s" s="0">
-        <v>98</v>
+        <v>123</v>
       </c>
       <c r="M2" t="s" s="0">
-        <v>60</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3">
@@ -571,19 +813,19 @@
         <v>1024.0</v>
       </c>
       <c r="I3" t="s" s="0">
-        <v>82</v>
+        <v>67</v>
       </c>
       <c r="J3" t="s" s="0">
-        <v>61</v>
+        <v>40</v>
       </c>
       <c r="K3" t="s" s="0">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="L3" t="s" s="0">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="M3" t="s" s="0">
-        <v>60</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4">
@@ -594,7 +836,7 @@
         <v>48</v>
       </c>
       <c r="C4" t="s" s="0">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="D4" t="s" s="0">
         <v>37</v>
@@ -612,19 +854,19 @@
         <v>1024.0</v>
       </c>
       <c r="I4" t="s" s="0">
-        <v>82</v>
+        <v>53</v>
       </c>
       <c r="J4" t="s" s="0">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="K4" t="s" s="0">
-        <v>112</v>
+        <v>199</v>
       </c>
       <c r="L4" t="s" s="0">
-        <v>113</v>
+        <v>200</v>
       </c>
       <c r="M4" t="s" s="0">
-        <v>60</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5">
@@ -632,10 +874,10 @@
         <v>34</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="C5" t="s" s="0">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="D5" t="s" s="0">
         <v>37</v>
@@ -653,19 +895,19 @@
         <v>1024.0</v>
       </c>
       <c r="I5" t="s" s="0">
-        <v>39</v>
+        <v>53</v>
       </c>
       <c r="J5" t="s" s="0">
         <v>40</v>
       </c>
       <c r="K5" t="s" s="0">
-        <v>54</v>
+        <v>180</v>
       </c>
       <c r="L5" t="s" s="0">
-        <v>55</v>
+        <v>181</v>
       </c>
       <c r="M5" t="s" s="0">
-        <v>41</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -729,7 +971,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -766,24 +1008,50 @@
         <v>34</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="E2" t="n" s="0">
         <v>569.0</v>
       </c>
       <c r="F2" t="s" s="0">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="G2" t="s" s="0">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="H2" t="s" s="0">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="0">
+        <v>34</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>64</v>
+      </c>
+      <c r="C3" t="s" s="0">
+        <v>65</v>
+      </c>
+      <c r="D3" t="s" s="0">
+        <v>62</v>
+      </c>
+      <c r="E3" t="n" s="0">
+        <v>2692.0</v>
+      </c>
+      <c r="F3" t="s" s="0">
+        <v>66</v>
+      </c>
+      <c r="G3" t="s" s="0">
+        <v>66</v>
+      </c>
+      <c r="H3" t="s" s="0">
         <v>41</v>
       </c>
     </row>
@@ -840,44 +1108,44 @@
         <v>569.0</v>
       </c>
       <c r="E2" t="s" s="0">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="F2" t="s" s="0">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="G2" t="s" s="0">
-        <v>96</v>
+        <v>121</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C3" t="n" s="0">
         <v>1024.0</v>
       </c>
       <c r="D3" t="n" s="0">
-        <v>569.0</v>
+        <v>2692.0</v>
       </c>
       <c r="E3" t="s" s="0">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="F3" t="s" s="0">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="G3" t="s" s="0">
-        <v>114</v>
+        <v>126</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="C4" t="n" s="0">
         <v>1024.0</v>
@@ -886,28 +1154,16 @@
         <v>569.0</v>
       </c>
       <c r="E4" t="s" s="0">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="F4" t="s" s="0">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="G4" t="s" s="0">
-        <v>117</v>
+        <v>190</v>
       </c>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
-  <sheetData/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Improved TH+WM+Dryer action menus CLI+GUI
</commit_message>
<xml_diff>
--- a/unit-sh/shsXl.xlsx
+++ b/unit-sh/shsXl.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="598" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1383" uniqueCount="398">
   <si>
     <t>TASK_ID</t>
   </si>
@@ -607,6 +607,609 @@
   </si>
   <si>
     <t>2025-08-23T21:10:34.687104718+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>TH004</t>
+  </si>
+  <si>
+    <t>Basement_Heater</t>
+  </si>
+  <si>
+    <t>2025-08-23T22:33:33.094106779+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-23T22:33:33.094120833+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>TH005</t>
+  </si>
+  <si>
+    <t>GND_Hall_Heater</t>
+  </si>
+  <si>
+    <t>2025-08-23T22:33:59.950458140+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-23T22:33:59.950466132+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>TH006</t>
+  </si>
+  <si>
+    <t>Dining_Room_Heater</t>
+  </si>
+  <si>
+    <t>2025-08-23T22:34:20.735020883+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-23T22:34:20.735030235+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>TH007</t>
+  </si>
+  <si>
+    <t>Main_Room_1_Heater</t>
+  </si>
+  <si>
+    <t>2025-08-23T22:36:01.652889515+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-23T22:36:01.652897644+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>TH008</t>
+  </si>
+  <si>
+    <t>Main_Room_2_Heater</t>
+  </si>
+  <si>
+    <t>2025-08-23T22:36:16.893236745+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-23T22:36:16.893244269+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>TH009</t>
+  </si>
+  <si>
+    <t>Main_Bath_Heater</t>
+  </si>
+  <si>
+    <t>2025-08-23T22:36:43.803723276+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-23T22:36:43.803731732+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>TH010</t>
+  </si>
+  <si>
+    <t>Master_Room_1_Heater</t>
+  </si>
+  <si>
+    <t>2025-08-23T23:34:08.462031117+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-23T23:34:08.462040007+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>TH011</t>
+  </si>
+  <si>
+    <t>Master_Room_2_Heater</t>
+  </si>
+  <si>
+    <t>2025-08-23T23:34:44.340765495+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-23T23:34:44.340772165+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>TH012</t>
+  </si>
+  <si>
+    <t>Master_Bathroom_Heater</t>
+  </si>
+  <si>
+    <t>2025-08-23T23:35:06.756410059+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-23T23:35:06.756418783+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>WASHING_MACHINE</t>
+  </si>
+  <si>
+    <t>WM001</t>
+  </si>
+  <si>
+    <t>Family_WM</t>
+  </si>
+  <si>
+    <t>LG</t>
+  </si>
+  <si>
+    <t>TwinWash</t>
+  </si>
+  <si>
+    <t>on, off, start, stop, status</t>
+  </si>
+  <si>
+    <t>2025-08-23T23:35:51.318518608+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-23T23:35:51.318536992+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>DRYER</t>
+  </si>
+  <si>
+    <t>DR001</t>
+  </si>
+  <si>
+    <t>Family_DR</t>
+  </si>
+  <si>
+    <t>Bosch</t>
+  </si>
+  <si>
+    <t>Series 6</t>
+  </si>
+  <si>
+    <t>2025-08-23T23:36:10.220887632+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-23T23:36:10.220901501+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T12:31:44.195950294+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T12:31:44.196070803+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T12:32:22.367463540+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T12:32:22.367562917+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T13:14:50.214744384+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T13:14:50.214936034+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T13:14:54.612821957+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T13:14:54.612915665+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T13:47:55.567054776+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T13:47:55.567298892+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T13:47:56.313620251+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T13:47:56.313805757+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T13:47:56.885005813+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T13:47:56.885261024+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T13:48:16.352406697+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T13:48:16.352471905+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T13:48:16.378474855+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T13:48:16.378573508+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T14:05:14.501057369+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T14:05:14.501372091+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T14:05:14.540440925+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T14:05:14.540559311+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T14:05:20.160282265+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T14:05:20.160378847+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T14:05:20.499194909+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T14:05:20.499291470+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T14:05:20.894884096+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T14:05:20.895011323+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T14:05:22.669671711+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T14:05:22.669751695+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T14:05:23.019753270+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T14:05:23.019820137+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T14:05:23.350891883+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T14:05:23.350979823+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T14:05:51.241903097+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T14:05:51.242003909+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T14:08:00.299160866+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T14:08:00.299641727+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T14:08:00.329920633+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T14:08:00.330057523+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T14:57:39.668719544+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T14:57:39.673737190+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T14:57:41.039395354+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T14:57:41.047234852+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T14:57:42.341610933+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T14:57:42.341879530+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T14:57:43.283128215+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T14:57:43.283243919+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T14:57:44.258456693+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T14:57:44.258858726+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T14:57:45.240572639+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T14:57:45.241143812+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T14:57:46.257176436+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T14:57:46.257349811+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T14:57:47.009673180+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T14:57:47.009897487+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T14:57:47.914365889+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T14:57:47.914554669+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T14:57:48.757158618+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T14:57:48.757295783+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T14:57:49.676175507+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T14:57:49.676338452+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T14:57:50.368036614+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T14:57:50.368219306+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T14:57:55.881580945+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T14:57:55.882386102+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T14:57:56.439246156+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T14:57:56.439417886+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T14:57:57.015863235+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T14:57:57.015949299+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T14:58:03.311405757+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T14:58:03.311752682+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T14:58:03.911506336+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T14:58:03.911828975+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T14:58:04.622235242+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T14:58:04.622322192+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T15:18:07.232548121+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T15:18:07.232728503+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T15:18:12.267168569+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T15:18:12.267302906+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T17:26:51.788464195+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T17:26:51.788573277+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T17:26:51.809859484+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T17:26:51.809916281+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T17:26:53.304393268+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T17:26:53.304450771+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T17:26:53.316955407+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T17:26:53.317004361+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T18:37:25.913172952+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T18:37:25.913641859+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T19:48:09.247330754+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T19:48:09.247526692+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T19:48:09.272222572+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T19:48:09.272299135+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T19:48:11.735503067+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T19:48:11.735560158+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T19:48:11.749300960+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T19:48:11.749362061+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T19:49:06.357791208+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T19:49:06.357978325+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T19:49:06.383439222+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T19:49:06.383500017+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T19:49:09.502539673+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T19:49:09.502818113+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T19:49:09.751002391+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T19:49:09.751057777+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T19:49:09.977267961+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T19:49:09.977326199+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T19:49:10.902327590+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T19:49:10.902623262+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T19:49:11.149589751+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T19:49:11.149638521+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T19:49:11.361672150+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T19:49:11.361726947+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T19:49:12.261164928+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T19:49:12.261319241+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T19:49:12.498870953+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T19:49:12.498933406+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T19:49:12.805364635+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T19:49:12.805424044+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T21:55:44.532963910+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T21:55:44.533710459+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T21:59:33.589312843+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T21:59:33.589460126+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T21:59:33.635523308+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T21:59:33.635664271+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T22:04:57.246187123+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T22:04:57.246272295+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T22:17:43.239558804+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T22:17:43.239747264+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T22:17:43.296492963+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T22:17:43.296593751+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T22:17:43.328811761+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T22:17:43.329117430+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T23:15:41.710787157+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T23:15:41.711169564+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T23:16:12.321124883+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T23:16:12.321420216+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T23:16:12.371465029+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T23:16:12.371657434+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T23:16:12.410964907+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T23:16:12.411091478+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T23:30:58.749353599+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T23:30:58.749581466+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T23:31:06.858184367+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T23:31:06.858399415+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T23:31:06.915971877+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T23:31:06.916564963+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T23:31:06.973341037+02:00[Europe/Amsterdam]</t>
+  </si>
+  <si>
+    <t>2025-08-24T23:31:06.973585571+02:00[Europe/Amsterdam]</t>
   </si>
 </sst>
 </file>
@@ -687,7 +1290,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:M15"/>
+  <dimension ref="A1:M26"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1135,10 +1738,10 @@
         <v>111</v>
       </c>
       <c r="K11" t="s" s="0">
-        <v>187</v>
+        <v>344</v>
       </c>
       <c r="L11" t="s" s="0">
-        <v>188</v>
+        <v>345</v>
       </c>
       <c r="M11" t="s" s="0">
         <v>109</v>
@@ -1211,16 +1814,16 @@
         <v>23.0</v>
       </c>
       <c r="I13" t="s" s="0">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="J13" t="s" s="0">
         <v>111</v>
       </c>
       <c r="K13" t="s" s="0">
-        <v>171</v>
+        <v>322</v>
       </c>
       <c r="L13" t="s" s="0">
-        <v>172</v>
+        <v>323</v>
       </c>
       <c r="M13" t="s" s="0">
         <v>109</v>
@@ -1284,7 +1887,7 @@
         <v>147</v>
       </c>
       <c r="F15" t="b" s="0">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G15" t="n" s="0">
         <v>23.0</v>
@@ -1293,18 +1896,469 @@
         <v>23.0</v>
       </c>
       <c r="I15" t="s" s="0">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="J15" t="s" s="0">
+        <v>64</v>
+      </c>
+      <c r="K15" t="s" s="0">
+        <v>286</v>
+      </c>
+      <c r="L15" t="s" s="0">
+        <v>287</v>
+      </c>
+      <c r="M15" t="s" s="0">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s" s="0">
+        <v>143</v>
+      </c>
+      <c r="B16" t="s" s="0">
+        <v>197</v>
+      </c>
+      <c r="C16" t="s" s="0">
+        <v>198</v>
+      </c>
+      <c r="D16" t="s" s="0">
+        <v>146</v>
+      </c>
+      <c r="E16" t="s" s="0">
+        <v>147</v>
+      </c>
+      <c r="F16" t="b" s="0">
+        <v>0</v>
+      </c>
+      <c r="G16" t="n" s="0">
+        <v>23.0</v>
+      </c>
+      <c r="H16" t="n" s="0">
+        <v>23.0</v>
+      </c>
+      <c r="I16" t="s" s="0">
+        <v>109</v>
+      </c>
+      <c r="J16" t="s" s="0">
+        <v>64</v>
+      </c>
+      <c r="K16" t="s" s="0">
+        <v>326</v>
+      </c>
+      <c r="L16" t="s" s="0">
+        <v>327</v>
+      </c>
+      <c r="M16" t="s" s="0">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s" s="0">
+        <v>143</v>
+      </c>
+      <c r="B17" t="s" s="0">
+        <v>201</v>
+      </c>
+      <c r="C17" t="s" s="0">
+        <v>202</v>
+      </c>
+      <c r="D17" t="s" s="0">
+        <v>146</v>
+      </c>
+      <c r="E17" t="s" s="0">
+        <v>147</v>
+      </c>
+      <c r="F17" t="b" s="0">
+        <v>0</v>
+      </c>
+      <c r="G17" t="n" s="0">
+        <v>23.0</v>
+      </c>
+      <c r="H17" t="n" s="0">
+        <v>23.0</v>
+      </c>
+      <c r="I17" t="s" s="0">
+        <v>148</v>
+      </c>
+      <c r="J17" t="s" s="0">
+        <v>64</v>
+      </c>
+      <c r="K17" t="s" s="0">
+        <v>203</v>
+      </c>
+      <c r="L17" t="s" s="0">
+        <v>204</v>
+      </c>
+      <c r="M17" t="s" s="0">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s" s="0">
+        <v>143</v>
+      </c>
+      <c r="B18" t="s" s="0">
+        <v>205</v>
+      </c>
+      <c r="C18" t="s" s="0">
+        <v>206</v>
+      </c>
+      <c r="D18" t="s" s="0">
+        <v>146</v>
+      </c>
+      <c r="E18" t="s" s="0">
+        <v>147</v>
+      </c>
+      <c r="F18" t="b" s="0">
+        <v>0</v>
+      </c>
+      <c r="G18" t="n" s="0">
+        <v>23.0</v>
+      </c>
+      <c r="H18" t="n" s="0">
+        <v>23.0</v>
+      </c>
+      <c r="I18" t="s" s="0">
+        <v>109</v>
+      </c>
+      <c r="J18" t="s" s="0">
+        <v>64</v>
+      </c>
+      <c r="K18" t="s" s="0">
+        <v>280</v>
+      </c>
+      <c r="L18" t="s" s="0">
+        <v>281</v>
+      </c>
+      <c r="M18" t="s" s="0">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s" s="0">
+        <v>143</v>
+      </c>
+      <c r="B19" t="s" s="0">
+        <v>209</v>
+      </c>
+      <c r="C19" t="s" s="0">
+        <v>210</v>
+      </c>
+      <c r="D19" t="s" s="0">
+        <v>146</v>
+      </c>
+      <c r="E19" t="s" s="0">
+        <v>147</v>
+      </c>
+      <c r="F19" t="b" s="0">
+        <v>0</v>
+      </c>
+      <c r="G19" t="n" s="0">
+        <v>23.0</v>
+      </c>
+      <c r="H19" t="n" s="0">
+        <v>23.0</v>
+      </c>
+      <c r="I19" t="s" s="0">
+        <v>109</v>
+      </c>
+      <c r="J19" t="s" s="0">
         <v>111</v>
       </c>
-      <c r="K15" t="s" s="0">
-        <v>164</v>
-      </c>
-      <c r="L15" t="s" s="0">
-        <v>165</v>
-      </c>
-      <c r="M15" t="s" s="0">
+      <c r="K19" t="s" s="0">
+        <v>366</v>
+      </c>
+      <c r="L19" t="s" s="0">
+        <v>367</v>
+      </c>
+      <c r="M19" t="s" s="0">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s" s="0">
+        <v>143</v>
+      </c>
+      <c r="B20" t="s" s="0">
+        <v>213</v>
+      </c>
+      <c r="C20" t="s" s="0">
+        <v>214</v>
+      </c>
+      <c r="D20" t="s" s="0">
+        <v>146</v>
+      </c>
+      <c r="E20" t="s" s="0">
+        <v>147</v>
+      </c>
+      <c r="F20" t="b" s="0">
+        <v>0</v>
+      </c>
+      <c r="G20" t="n" s="0">
+        <v>23.0</v>
+      </c>
+      <c r="H20" t="n" s="0">
+        <v>23.0</v>
+      </c>
+      <c r="I20" t="s" s="0">
+        <v>148</v>
+      </c>
+      <c r="J20" t="s" s="0">
+        <v>64</v>
+      </c>
+      <c r="K20" t="s" s="0">
+        <v>215</v>
+      </c>
+      <c r="L20" t="s" s="0">
+        <v>216</v>
+      </c>
+      <c r="M20" t="s" s="0">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s" s="0">
+        <v>143</v>
+      </c>
+      <c r="B21" t="s" s="0">
+        <v>217</v>
+      </c>
+      <c r="C21" t="s" s="0">
+        <v>218</v>
+      </c>
+      <c r="D21" t="s" s="0">
+        <v>146</v>
+      </c>
+      <c r="E21" t="s" s="0">
+        <v>147</v>
+      </c>
+      <c r="F21" t="b" s="0">
+        <v>0</v>
+      </c>
+      <c r="G21" t="n" s="0">
+        <v>23.0</v>
+      </c>
+      <c r="H21" t="n" s="0">
+        <v>23.0</v>
+      </c>
+      <c r="I21" t="s" s="0">
+        <v>148</v>
+      </c>
+      <c r="J21" t="s" s="0">
+        <v>64</v>
+      </c>
+      <c r="K21" t="s" s="0">
+        <v>219</v>
+      </c>
+      <c r="L21" t="s" s="0">
+        <v>220</v>
+      </c>
+      <c r="M21" t="s" s="0">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s" s="0">
+        <v>143</v>
+      </c>
+      <c r="B22" t="s" s="0">
+        <v>221</v>
+      </c>
+      <c r="C22" t="s" s="0">
+        <v>222</v>
+      </c>
+      <c r="D22" t="s" s="0">
+        <v>146</v>
+      </c>
+      <c r="E22" t="s" s="0">
+        <v>147</v>
+      </c>
+      <c r="F22" t="b" s="0">
+        <v>0</v>
+      </c>
+      <c r="G22" t="n" s="0">
+        <v>23.0</v>
+      </c>
+      <c r="H22" t="n" s="0">
+        <v>23.0</v>
+      </c>
+      <c r="I22" t="s" s="0">
+        <v>109</v>
+      </c>
+      <c r="J22" t="s" s="0">
+        <v>111</v>
+      </c>
+      <c r="K22" t="s" s="0">
+        <v>372</v>
+      </c>
+      <c r="L22" t="s" s="0">
+        <v>373</v>
+      </c>
+      <c r="M22" t="s" s="0">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s" s="0">
+        <v>143</v>
+      </c>
+      <c r="B23" t="s" s="0">
+        <v>225</v>
+      </c>
+      <c r="C23" t="s" s="0">
+        <v>226</v>
+      </c>
+      <c r="D23" t="s" s="0">
+        <v>146</v>
+      </c>
+      <c r="E23" t="s" s="0">
+        <v>147</v>
+      </c>
+      <c r="F23" t="b" s="0">
+        <v>0</v>
+      </c>
+      <c r="G23" t="n" s="0">
+        <v>23.0</v>
+      </c>
+      <c r="H23" t="n" s="0">
+        <v>23.0</v>
+      </c>
+      <c r="I23" t="s" s="0">
+        <v>109</v>
+      </c>
+      <c r="J23" t="s" s="0">
+        <v>64</v>
+      </c>
+      <c r="K23" t="s" s="0">
+        <v>334</v>
+      </c>
+      <c r="L23" t="s" s="0">
+        <v>335</v>
+      </c>
+      <c r="M23" t="s" s="0">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s" s="0">
+        <v>143</v>
+      </c>
+      <c r="B24" t="s" s="0">
+        <v>229</v>
+      </c>
+      <c r="C24" t="s" s="0">
+        <v>230</v>
+      </c>
+      <c r="D24" t="s" s="0">
+        <v>146</v>
+      </c>
+      <c r="E24" t="s" s="0">
+        <v>147</v>
+      </c>
+      <c r="F24" t="b" s="0">
+        <v>0</v>
+      </c>
+      <c r="G24" t="n" s="0">
+        <v>23.0</v>
+      </c>
+      <c r="H24" t="n" s="0">
+        <v>23.0</v>
+      </c>
+      <c r="I24" t="s" s="0">
+        <v>148</v>
+      </c>
+      <c r="J24" t="s" s="0">
+        <v>64</v>
+      </c>
+      <c r="K24" t="s" s="0">
+        <v>231</v>
+      </c>
+      <c r="L24" t="s" s="0">
+        <v>232</v>
+      </c>
+      <c r="M24" t="s" s="0">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s" s="0">
+        <v>233</v>
+      </c>
+      <c r="B25" t="s" s="0">
+        <v>234</v>
+      </c>
+      <c r="C25" t="s" s="0">
+        <v>235</v>
+      </c>
+      <c r="D25" t="s" s="0">
+        <v>236</v>
+      </c>
+      <c r="E25" t="s" s="0">
+        <v>237</v>
+      </c>
+      <c r="F25" t="b" s="0">
+        <v>0</v>
+      </c>
+      <c r="G25" t="n" s="0">
+        <v>1024.0</v>
+      </c>
+      <c r="H25" t="n" s="0">
+        <v>1024.0</v>
+      </c>
+      <c r="I25" t="s" s="0">
+        <v>109</v>
+      </c>
+      <c r="J25" t="s" s="0">
+        <v>64</v>
+      </c>
+      <c r="K25" t="s" s="0">
+        <v>368</v>
+      </c>
+      <c r="L25" t="s" s="0">
+        <v>369</v>
+      </c>
+      <c r="M25" t="s" s="0">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s" s="0">
+        <v>241</v>
+      </c>
+      <c r="B26" t="s" s="0">
+        <v>242</v>
+      </c>
+      <c r="C26" t="s" s="0">
+        <v>243</v>
+      </c>
+      <c r="D26" t="s" s="0">
+        <v>244</v>
+      </c>
+      <c r="E26" t="s" s="0">
+        <v>245</v>
+      </c>
+      <c r="F26" t="b" s="0">
+        <v>0</v>
+      </c>
+      <c r="G26" t="n" s="0">
+        <v>1024.0</v>
+      </c>
+      <c r="H26" t="n" s="0">
+        <v>1024.0</v>
+      </c>
+      <c r="I26" t="s" s="0">
+        <v>109</v>
+      </c>
+      <c r="J26" t="s" s="0">
+        <v>64</v>
+      </c>
+      <c r="K26" t="s" s="0">
+        <v>396</v>
+      </c>
+      <c r="L26" t="s" s="0">
+        <v>397</v>
+      </c>
+      <c r="M26" t="s" s="0">
         <v>109</v>
       </c>
     </row>
@@ -1642,29 +2696,6 @@
         <v>140</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="s" s="0">
-        <v>155</v>
-      </c>
-      <c r="B4" t="s" s="0">
-        <v>156</v>
-      </c>
-      <c r="C4" t="n" s="0">
-        <v>23.0</v>
-      </c>
-      <c r="D4" t="n" s="0">
-        <v>22.0</v>
-      </c>
-      <c r="E4" t="s" s="0">
-        <v>36</v>
-      </c>
-      <c r="F4" t="s" s="0">
-        <v>35</v>
-      </c>
-      <c r="G4" t="s" s="0">
-        <v>163</v>
-      </c>
-    </row>
     <row r="5">
       <c r="A5" t="s" s="0">
         <v>151</v>

</xml_diff>